<commit_message>
1st prototyp of Chada class
</commit_message>
<xml_diff>
--- a/documents/Raman data formats.xlsx
+++ b/documents/Raman data formats.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\barton\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\vm-stor-51\alle\Projekte Kunststoffe\RD\MA\Öffentliche_Projekte\2020-01-07_230007_H2020-CHARISMA_barton\Python\charisma-raman-spectrum-harmonization\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1232" uniqueCount="514">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1237" uniqueCount="515">
   <si>
     <t>Renishaw InVia</t>
   </si>
@@ -1574,13 +1574,16 @@
   </si>
   <si>
     <t>txt</t>
+  </si>
+  <si>
+    <t>Export single sspectra or maps to .spc by right-click</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1707,8 +1710,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1724,6 +1734,11 @@
       <patternFill patternType="solid">
         <fgColor theme="2"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
   </fills>
@@ -1792,15 +1807,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="6">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1870,15 +1886,6 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1891,15 +1898,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1917,12 +1915,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1931,9 +1923,6 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1943,12 +1932,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1968,12 +1951,6 @@
     <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1983,19 +1960,7 @@
     <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="4" applyBorder="1" applyAlignment="1">
@@ -2016,11 +1981,64 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="6"/>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="7">
     <cellStyle name="Gut" xfId="4" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="2"/>
     <cellStyle name="Link" xfId="5" builtinId="8"/>
+    <cellStyle name="Neutral" xfId="6" builtinId="28"/>
     <cellStyle name="Normal 2" xfId="3"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
     <cellStyle name="Standard 2" xfId="1"/>
@@ -2395,8 +2413,8 @@
   </sheetPr>
   <dimension ref="A1:K40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2442,367 +2460,377 @@
       </c>
     </row>
     <row r="2" spans="1:11" s="16" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A2" s="40">
+      <c r="A2" s="34">
         <v>1</v>
       </c>
       <c r="B2" s="22" t="s">
         <v>90</v>
       </c>
-      <c r="C2" s="55" t="s">
+      <c r="C2" s="46" t="s">
         <v>14</v>
       </c>
       <c r="D2" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="E2" s="41" t="s">
+      <c r="E2" s="35" t="s">
         <v>94</v>
       </c>
-      <c r="F2" s="74" t="s">
+      <c r="F2" s="57" t="s">
         <v>60</v>
       </c>
-      <c r="G2" s="75"/>
-      <c r="H2" s="74" t="s">
+      <c r="G2" s="58"/>
+      <c r="H2" s="57" t="s">
         <v>60</v>
       </c>
-      <c r="I2" s="42"/>
-      <c r="J2" s="43" t="s">
+      <c r="I2" s="36"/>
+      <c r="J2" s="37" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="44">
+      <c r="A3" s="62">
         <v>2</v>
       </c>
-      <c r="B3" s="35" t="s">
+      <c r="B3" s="65" t="s">
         <v>90</v>
       </c>
-      <c r="C3" s="56" t="s">
+      <c r="C3" s="70" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="36" t="s">
+      <c r="D3" s="69" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="45" t="s">
+      <c r="E3" s="73" t="s">
         <v>69</v>
       </c>
       <c r="F3" s="71" t="s">
         <v>60</v>
       </c>
-      <c r="G3" s="76"/>
-      <c r="H3" s="76"/>
-      <c r="I3" s="46"/>
-      <c r="J3" s="47"/>
-      <c r="K3" s="33"/>
+      <c r="G3" s="59"/>
+      <c r="H3" s="59"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="39"/>
+      <c r="K3" s="30"/>
     </row>
     <row r="4" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="44"/>
-      <c r="B4" s="35"/>
-      <c r="C4" s="56"/>
-      <c r="D4" s="36"/>
-      <c r="E4" s="45"/>
+      <c r="A4" s="62"/>
+      <c r="B4" s="65"/>
+      <c r="C4" s="70"/>
+      <c r="D4" s="69"/>
+      <c r="E4" s="73"/>
       <c r="F4" s="72"/>
-      <c r="G4" s="76"/>
-      <c r="H4" s="76"/>
-      <c r="I4" s="46"/>
-      <c r="J4" s="47"/>
-      <c r="K4" s="33"/>
+      <c r="G4" s="59"/>
+      <c r="H4" s="59"/>
+      <c r="I4" s="38"/>
+      <c r="J4" s="39"/>
+      <c r="K4" s="30"/>
     </row>
     <row r="5" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="44"/>
-      <c r="B5" s="35"/>
-      <c r="C5" s="56"/>
-      <c r="D5" s="36"/>
-      <c r="E5" s="48" t="s">
+      <c r="A5" s="62"/>
+      <c r="B5" s="65"/>
+      <c r="C5" s="70"/>
+      <c r="D5" s="69"/>
+      <c r="E5" s="40" t="s">
         <v>70</v>
       </c>
-      <c r="F5" s="73" t="s">
+      <c r="F5" s="56" t="s">
         <v>60</v>
       </c>
-      <c r="G5" s="76"/>
-      <c r="H5" s="73" t="s">
+      <c r="G5" s="59"/>
+      <c r="H5" s="56" t="s">
         <v>60</v>
       </c>
       <c r="I5" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="J5" s="47"/>
-      <c r="K5" s="33"/>
+      <c r="J5" s="39"/>
+      <c r="K5" s="30"/>
     </row>
     <row r="6" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="44"/>
-      <c r="B6" s="35"/>
-      <c r="C6" s="56"/>
-      <c r="D6" s="36"/>
-      <c r="E6" s="48" t="s">
+      <c r="A6" s="62"/>
+      <c r="B6" s="65"/>
+      <c r="C6" s="70"/>
+      <c r="D6" s="69"/>
+      <c r="E6" s="40" t="s">
         <v>71</v>
       </c>
-      <c r="F6" s="73" t="s">
+      <c r="F6" s="56" t="s">
         <v>60</v>
       </c>
-      <c r="G6" s="76"/>
-      <c r="H6" s="76"/>
-      <c r="I6" s="46"/>
-      <c r="J6" s="47"/>
-      <c r="K6" s="33"/>
+      <c r="G6" s="59"/>
+      <c r="H6" s="59"/>
+      <c r="I6" s="38"/>
+      <c r="J6" s="39"/>
+      <c r="K6" s="30"/>
     </row>
     <row r="7" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="44"/>
-      <c r="B7" s="35"/>
-      <c r="C7" s="56"/>
-      <c r="D7" s="36"/>
-      <c r="E7" s="48" t="s">
+      <c r="A7" s="62"/>
+      <c r="B7" s="65"/>
+      <c r="C7" s="70"/>
+      <c r="D7" s="69"/>
+      <c r="E7" s="40" t="s">
         <v>72</v>
       </c>
-      <c r="F7" s="76"/>
-      <c r="G7" s="76"/>
-      <c r="H7" s="76"/>
-      <c r="I7" s="46"/>
-      <c r="J7" s="47"/>
-      <c r="K7" s="33"/>
+      <c r="F7" s="59"/>
+      <c r="G7" s="59"/>
+      <c r="H7" s="59"/>
+      <c r="I7" s="38"/>
+      <c r="J7" s="39"/>
+      <c r="K7" s="30"/>
     </row>
     <row r="8" spans="1:11" s="16" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A8" s="44"/>
-      <c r="B8" s="35"/>
-      <c r="C8" s="56"/>
-      <c r="D8" s="36"/>
-      <c r="E8" s="48" t="s">
+      <c r="A8" s="62"/>
+      <c r="B8" s="65"/>
+      <c r="C8" s="70"/>
+      <c r="D8" s="69"/>
+      <c r="E8" s="40" t="s">
         <v>97</v>
       </c>
-      <c r="F8" s="73" t="s">
+      <c r="F8" s="56" t="s">
         <v>60</v>
       </c>
-      <c r="G8" s="77" t="s">
+      <c r="G8" s="60" t="s">
         <v>506</v>
       </c>
-      <c r="H8" s="73" t="s">
+      <c r="H8" s="56" t="s">
         <v>60</v>
       </c>
       <c r="I8" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="J8" s="49"/>
-      <c r="K8" s="33"/>
+      <c r="J8" s="41"/>
+      <c r="K8" s="30"/>
     </row>
     <row r="9" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="44"/>
-      <c r="B9" s="35"/>
-      <c r="C9" s="56"/>
-      <c r="D9" s="36"/>
-      <c r="E9" s="48" t="s">
+      <c r="A9" s="62"/>
+      <c r="B9" s="65"/>
+      <c r="C9" s="70"/>
+      <c r="D9" s="69"/>
+      <c r="E9" s="40" t="s">
         <v>73</v>
       </c>
-      <c r="F9" s="76"/>
-      <c r="G9" s="76"/>
-      <c r="H9" s="76"/>
-      <c r="I9" s="46"/>
-      <c r="J9" s="47"/>
-      <c r="K9" s="33"/>
+      <c r="F9" s="59"/>
+      <c r="G9" s="59"/>
+      <c r="H9" s="59"/>
+      <c r="I9" s="38"/>
+      <c r="J9" s="39"/>
+      <c r="K9" s="30"/>
     </row>
     <row r="10" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="50">
+      <c r="A10" s="63">
         <v>3</v>
       </c>
-      <c r="B10" s="28" t="s">
+      <c r="B10" s="66" t="s">
         <v>90</v>
       </c>
-      <c r="C10" s="57" t="s">
+      <c r="C10" s="74" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="27" t="s">
+      <c r="D10" s="75" t="s">
         <v>28</v>
       </c>
-      <c r="E10" s="51" t="s">
+      <c r="E10" s="42" t="s">
         <v>82</v>
       </c>
-      <c r="F10" s="78"/>
-      <c r="G10" s="78"/>
-      <c r="H10" s="78"/>
-      <c r="I10" s="52"/>
-      <c r="J10" s="43"/>
+      <c r="F10" s="61"/>
+      <c r="G10" s="61"/>
+      <c r="H10" s="61"/>
+      <c r="I10" s="43"/>
+      <c r="J10" s="37"/>
     </row>
     <row r="11" spans="1:11" s="16" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A11" s="50"/>
-      <c r="B11" s="28"/>
-      <c r="C11" s="57"/>
-      <c r="D11" s="27"/>
-      <c r="E11" s="51" t="s">
+      <c r="A11" s="63"/>
+      <c r="B11" s="66"/>
+      <c r="C11" s="74"/>
+      <c r="D11" s="75"/>
+      <c r="E11" s="42" t="s">
         <v>77</v>
       </c>
-      <c r="F11" s="78"/>
-      <c r="G11" s="78"/>
-      <c r="H11" s="73" t="s">
+      <c r="F11" s="61"/>
+      <c r="G11" s="61"/>
+      <c r="H11" s="56" t="s">
         <v>60</v>
       </c>
-      <c r="I11" s="52"/>
-      <c r="J11" s="43"/>
+      <c r="I11" s="43"/>
+      <c r="J11" s="37"/>
     </row>
     <row r="12" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="50"/>
-      <c r="B12" s="28"/>
-      <c r="C12" s="57"/>
-      <c r="D12" s="27"/>
-      <c r="E12" s="51" t="s">
+      <c r="A12" s="63"/>
+      <c r="B12" s="66"/>
+      <c r="C12" s="74"/>
+      <c r="D12" s="75"/>
+      <c r="E12" s="42" t="s">
         <v>78</v>
       </c>
-      <c r="F12" s="78"/>
-      <c r="G12" s="78"/>
-      <c r="H12" s="73" t="s">
+      <c r="F12" s="61"/>
+      <c r="G12" s="61"/>
+      <c r="H12" s="56" t="s">
         <v>60</v>
       </c>
-      <c r="I12" s="52"/>
-      <c r="J12" s="43"/>
+      <c r="I12" s="43"/>
+      <c r="J12" s="37"/>
     </row>
     <row r="13" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="50"/>
-      <c r="B13" s="28"/>
-      <c r="C13" s="57"/>
-      <c r="D13" s="27"/>
-      <c r="E13" s="51" t="s">
+      <c r="A13" s="63"/>
+      <c r="B13" s="66"/>
+      <c r="C13" s="74"/>
+      <c r="D13" s="75"/>
+      <c r="E13" s="42" t="s">
         <v>79</v>
       </c>
-      <c r="F13" s="78"/>
-      <c r="G13" s="78"/>
-      <c r="H13" s="78"/>
-      <c r="I13" s="52"/>
-      <c r="J13" s="43"/>
+      <c r="F13" s="61"/>
+      <c r="G13" s="61"/>
+      <c r="H13" s="61"/>
+      <c r="I13" s="43"/>
+      <c r="J13" s="37"/>
     </row>
     <row r="14" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="50"/>
-      <c r="B14" s="28"/>
-      <c r="C14" s="57"/>
-      <c r="D14" s="27"/>
-      <c r="E14" s="51" t="s">
+      <c r="A14" s="63"/>
+      <c r="B14" s="66"/>
+      <c r="C14" s="74"/>
+      <c r="D14" s="75"/>
+      <c r="E14" s="42" t="s">
         <v>80</v>
       </c>
-      <c r="F14" s="78"/>
-      <c r="G14" s="78"/>
-      <c r="H14" s="78"/>
-      <c r="I14" s="52"/>
-      <c r="J14" s="43"/>
+      <c r="F14" s="61"/>
+      <c r="G14" s="61"/>
+      <c r="H14" s="61"/>
+      <c r="I14" s="43"/>
+      <c r="J14" s="37"/>
     </row>
     <row r="15" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="50"/>
-      <c r="B15" s="28"/>
-      <c r="C15" s="57"/>
-      <c r="D15" s="27"/>
-      <c r="E15" s="51" t="s">
+      <c r="A15" s="63"/>
+      <c r="B15" s="66"/>
+      <c r="C15" s="74"/>
+      <c r="D15" s="75"/>
+      <c r="E15" s="42" t="s">
         <v>81</v>
       </c>
-      <c r="F15" s="78"/>
-      <c r="G15" s="78"/>
-      <c r="H15" s="73" t="s">
+      <c r="F15" s="61"/>
+      <c r="G15" s="61"/>
+      <c r="H15" s="56" t="s">
         <v>60</v>
       </c>
-      <c r="I15" s="52"/>
-      <c r="J15" s="43"/>
+      <c r="I15" s="43"/>
+      <c r="J15" s="37"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A16" s="53">
+      <c r="A16" s="44">
         <v>4</v>
       </c>
-      <c r="B16" s="30" t="s">
+      <c r="B16" s="27" t="s">
         <v>90</v>
       </c>
-      <c r="C16" s="58" t="s">
+      <c r="C16" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="D16" s="31" t="s">
+      <c r="D16" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="E16" s="54" t="s">
+      <c r="E16" s="45" t="s">
         <v>96</v>
       </c>
-      <c r="F16" s="49"/>
-      <c r="G16" s="49"/>
-      <c r="H16" s="49"/>
-      <c r="I16" s="49"/>
-      <c r="J16" s="47"/>
-      <c r="K16" s="33"/>
+      <c r="F16" s="79" t="s">
+        <v>443</v>
+      </c>
+      <c r="G16" s="31" t="s">
+        <v>31</v>
+      </c>
+      <c r="H16" s="56" t="s">
+        <v>60</v>
+      </c>
+      <c r="I16" s="56" t="s">
+        <v>60</v>
+      </c>
+      <c r="J16" s="39" t="s">
+        <v>514</v>
+      </c>
+      <c r="K16" s="30"/>
     </row>
     <row r="17" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="53">
+      <c r="A17" s="44">
         <v>5</v>
       </c>
       <c r="B17" s="22" t="s">
         <v>90</v>
       </c>
-      <c r="C17" s="55" t="s">
+      <c r="C17" s="46" t="s">
         <v>18</v>
       </c>
       <c r="D17" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="E17" s="41" t="s">
+      <c r="E17" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="F17" s="42"/>
-      <c r="G17" s="42"/>
-      <c r="H17" s="42"/>
-      <c r="I17" s="42"/>
-      <c r="J17" s="43"/>
+      <c r="F17" s="36"/>
+      <c r="G17" s="36"/>
+      <c r="H17" s="36"/>
+      <c r="I17" s="36"/>
+      <c r="J17" s="37"/>
     </row>
     <row r="18" spans="1:11" s="16" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A18" s="53">
+      <c r="A18" s="44">
         <v>6</v>
       </c>
-      <c r="B18" s="30" t="s">
+      <c r="B18" s="27" t="s">
         <v>90</v>
       </c>
-      <c r="C18" s="58" t="s">
+      <c r="C18" s="47" t="s">
         <v>19</v>
       </c>
-      <c r="D18" s="31" t="s">
+      <c r="D18" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="E18" s="54" t="s">
+      <c r="E18" s="45" t="s">
         <v>510</v>
       </c>
       <c r="F18" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="G18" s="47" t="s">
+      <c r="G18" s="39" t="s">
         <v>509</v>
       </c>
-      <c r="H18" s="49"/>
-      <c r="I18" s="49"/>
-      <c r="J18" s="47"/>
-      <c r="K18" s="33"/>
+      <c r="H18" s="41"/>
+      <c r="I18" s="41"/>
+      <c r="J18" s="39"/>
+      <c r="K18" s="30"/>
     </row>
     <row r="19" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="53">
+      <c r="A19" s="44">
         <v>8</v>
       </c>
-      <c r="B19" s="30" t="s">
+      <c r="B19" s="27" t="s">
         <v>90</v>
       </c>
-      <c r="C19" s="58" t="s">
+      <c r="C19" s="47" t="s">
         <v>17</v>
       </c>
-      <c r="D19" s="31" t="s">
+      <c r="D19" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="E19" s="32" t="s">
+      <c r="E19" s="29" t="s">
         <v>30</v>
       </c>
       <c r="F19" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="G19" s="34" t="s">
+      <c r="G19" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="H19" s="33"/>
-      <c r="I19" s="33"/>
-      <c r="J19" s="34"/>
-      <c r="K19" s="33"/>
+      <c r="H19" s="30"/>
+      <c r="I19" s="30"/>
+      <c r="J19" s="31"/>
+      <c r="K19" s="30"/>
     </row>
     <row r="20" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="53">
+      <c r="A20" s="44">
         <v>9</v>
       </c>
-      <c r="B20" s="61" t="s">
+      <c r="B20" s="50" t="s">
         <v>91</v>
       </c>
-      <c r="C20" s="62" t="s">
+      <c r="C20" s="51" t="s">
         <v>61</v>
       </c>
       <c r="D20" s="23" t="s">
@@ -2814,109 +2842,109 @@
       <c r="J20" s="17"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A21" s="53">
+      <c r="A21" s="44">
         <v>10</v>
       </c>
-      <c r="B21" s="59" t="s">
+      <c r="B21" s="48" t="s">
         <v>91</v>
       </c>
-      <c r="C21" s="60" t="s">
+      <c r="C21" s="49" t="s">
         <v>36</v>
       </c>
-      <c r="D21" s="31"/>
-      <c r="E21" s="32" t="s">
+      <c r="D21" s="28"/>
+      <c r="E21" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="F21" s="33"/>
-      <c r="G21" s="33"/>
-      <c r="H21" s="33"/>
-      <c r="I21" s="33"/>
-      <c r="J21" s="34"/>
-      <c r="K21" s="33"/>
+      <c r="F21" s="30"/>
+      <c r="G21" s="30"/>
+      <c r="H21" s="30"/>
+      <c r="I21" s="30"/>
+      <c r="J21" s="31"/>
+      <c r="K21" s="30"/>
     </row>
     <row r="22" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="69">
+      <c r="A22" s="64">
         <v>11</v>
       </c>
-      <c r="B22" s="63" t="s">
+      <c r="B22" s="67" t="s">
         <v>91</v>
       </c>
-      <c r="C22" s="64" t="s">
+      <c r="C22" s="76" t="s">
         <v>64</v>
       </c>
-      <c r="D22" s="37"/>
+      <c r="D22" s="77"/>
       <c r="E22" s="17" t="s">
         <v>88</v>
       </c>
       <c r="J22" s="17"/>
     </row>
     <row r="23" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="69"/>
-      <c r="B23" s="63"/>
-      <c r="C23" s="64"/>
-      <c r="D23" s="37"/>
+      <c r="A23" s="64"/>
+      <c r="B23" s="67"/>
+      <c r="C23" s="76"/>
+      <c r="D23" s="77"/>
       <c r="E23" s="17" t="s">
         <v>84</v>
       </c>
       <c r="J23" s="17"/>
     </row>
     <row r="24" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="69"/>
-      <c r="B24" s="63"/>
-      <c r="C24" s="64"/>
-      <c r="D24" s="37"/>
+      <c r="A24" s="64"/>
+      <c r="B24" s="67"/>
+      <c r="C24" s="76"/>
+      <c r="D24" s="77"/>
       <c r="E24" s="17" t="s">
         <v>85</v>
       </c>
       <c r="J24" s="17"/>
     </row>
     <row r="25" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="69"/>
-      <c r="B25" s="63"/>
-      <c r="C25" s="64"/>
-      <c r="D25" s="37"/>
+      <c r="A25" s="64"/>
+      <c r="B25" s="67"/>
+      <c r="C25" s="76"/>
+      <c r="D25" s="77"/>
       <c r="E25" s="17" t="s">
         <v>86</v>
       </c>
       <c r="J25" s="17"/>
     </row>
     <row r="26" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="69"/>
-      <c r="B26" s="63"/>
-      <c r="C26" s="64"/>
-      <c r="D26" s="37"/>
+      <c r="A26" s="64"/>
+      <c r="B26" s="67"/>
+      <c r="C26" s="76"/>
+      <c r="D26" s="77"/>
       <c r="E26" s="17" t="s">
         <v>87</v>
       </c>
       <c r="J26" s="17"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A27" s="70">
+      <c r="A27" s="55">
         <v>12</v>
       </c>
-      <c r="B27" s="59" t="s">
+      <c r="B27" s="48" t="s">
         <v>91</v>
       </c>
-      <c r="C27" s="60" t="s">
+      <c r="C27" s="49" t="s">
         <v>46</v>
       </c>
-      <c r="D27" s="31"/>
-      <c r="E27" s="34"/>
-      <c r="F27" s="33"/>
-      <c r="G27" s="33"/>
-      <c r="H27" s="33"/>
-      <c r="I27" s="33"/>
-      <c r="J27" s="34"/>
-      <c r="K27" s="33"/>
+      <c r="D27" s="28"/>
+      <c r="E27" s="31"/>
+      <c r="F27" s="30"/>
+      <c r="G27" s="30"/>
+      <c r="H27" s="30"/>
+      <c r="I27" s="30"/>
+      <c r="J27" s="31"/>
+      <c r="K27" s="30"/>
     </row>
     <row r="28" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="70">
+      <c r="A28" s="55">
         <v>13</v>
       </c>
-      <c r="B28" s="61" t="s">
+      <c r="B28" s="50" t="s">
         <v>91</v>
       </c>
-      <c r="C28" s="62" t="s">
+      <c r="C28" s="51" t="s">
         <v>57</v>
       </c>
       <c r="D28" s="23" t="s">
@@ -2928,62 +2956,62 @@
       <c r="J28" s="17"/>
     </row>
     <row r="29" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="53">
+      <c r="A29" s="44">
         <v>7</v>
       </c>
       <c r="B29" s="18" t="s">
         <v>91</v>
       </c>
-      <c r="C29" s="65" t="s">
+      <c r="C29" s="52" t="s">
         <v>55</v>
       </c>
       <c r="D29" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="E29" s="41" t="s">
+      <c r="E29" s="35" t="s">
         <v>66</v>
       </c>
       <c r="F29" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="G29" s="43" t="s">
+      <c r="G29" s="37" t="s">
         <v>508</v>
       </c>
       <c r="H29" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="I29" s="42" t="s">
+      <c r="I29" s="36" t="s">
         <v>511</v>
       </c>
-      <c r="J29" s="43"/>
+      <c r="J29" s="37"/>
     </row>
     <row r="30" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="70">
+      <c r="A30" s="55">
         <v>14</v>
       </c>
-      <c r="B30" s="38" t="s">
+      <c r="B30" s="32" t="s">
         <v>92</v>
       </c>
-      <c r="C30" s="66" t="s">
+      <c r="C30" s="53" t="s">
         <v>47</v>
       </c>
-      <c r="D30" s="31"/>
-      <c r="E30" s="32"/>
-      <c r="F30" s="33"/>
-      <c r="G30" s="33"/>
-      <c r="H30" s="33"/>
-      <c r="I30" s="33"/>
-      <c r="J30" s="34"/>
-      <c r="K30" s="33"/>
+      <c r="D30" s="28"/>
+      <c r="E30" s="29"/>
+      <c r="F30" s="30"/>
+      <c r="G30" s="30"/>
+      <c r="H30" s="30"/>
+      <c r="I30" s="30"/>
+      <c r="J30" s="31"/>
+      <c r="K30" s="30"/>
     </row>
     <row r="31" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="70">
+      <c r="A31" s="55">
         <v>15</v>
       </c>
-      <c r="B31" s="39" t="s">
+      <c r="B31" s="33" t="s">
         <v>92</v>
       </c>
-      <c r="C31" s="67" t="s">
+      <c r="C31" s="54" t="s">
         <v>34</v>
       </c>
       <c r="D31" s="23"/>
@@ -2996,34 +3024,34 @@
       <c r="J31" s="17"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A32" s="70">
+      <c r="A32" s="55">
         <v>16</v>
       </c>
-      <c r="B32" s="38" t="s">
+      <c r="B32" s="32" t="s">
         <v>92</v>
       </c>
-      <c r="C32" s="66" t="s">
+      <c r="C32" s="53" t="s">
         <v>38</v>
       </c>
-      <c r="D32" s="31"/>
-      <c r="E32" s="32" t="s">
+      <c r="D32" s="28"/>
+      <c r="E32" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="F32" s="33"/>
-      <c r="G32" s="33"/>
-      <c r="H32" s="33"/>
-      <c r="I32" s="33"/>
-      <c r="J32" s="34"/>
-      <c r="K32" s="33"/>
+      <c r="F32" s="30"/>
+      <c r="G32" s="30"/>
+      <c r="H32" s="30"/>
+      <c r="I32" s="30"/>
+      <c r="J32" s="31"/>
+      <c r="K32" s="30"/>
     </row>
     <row r="33" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="70">
+      <c r="A33" s="55">
         <v>17</v>
       </c>
-      <c r="B33" s="39" t="s">
+      <c r="B33" s="33" t="s">
         <v>92</v>
       </c>
-      <c r="C33" s="67" t="s">
+      <c r="C33" s="54" t="s">
         <v>42</v>
       </c>
       <c r="D33" s="23"/>
@@ -3033,33 +3061,33 @@
       <c r="J33" s="17"/>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A34" s="70">
+      <c r="A34" s="55">
         <v>18</v>
       </c>
-      <c r="B34" s="38" t="s">
+      <c r="B34" s="32" t="s">
         <v>92</v>
       </c>
-      <c r="C34" s="66" t="s">
+      <c r="C34" s="53" t="s">
         <v>43</v>
       </c>
-      <c r="D34" s="31"/>
-      <c r="E34" s="34"/>
-      <c r="F34" s="33"/>
-      <c r="G34" s="33"/>
-      <c r="H34" s="33"/>
-      <c r="I34" s="33"/>
-      <c r="J34" s="34"/>
-      <c r="K34" s="33"/>
+      <c r="D34" s="28"/>
+      <c r="E34" s="31"/>
+      <c r="F34" s="30"/>
+      <c r="G34" s="30"/>
+      <c r="H34" s="30"/>
+      <c r="I34" s="30"/>
+      <c r="J34" s="31"/>
+      <c r="K34" s="30"/>
     </row>
     <row r="35" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="70">
+      <c r="A35" s="55">
         <v>19</v>
       </c>
-      <c r="B35" s="39"/>
+      <c r="B35" s="33"/>
       <c r="C35" s="68" t="s">
         <v>44</v>
       </c>
-      <c r="D35" s="36"/>
+      <c r="D35" s="69"/>
       <c r="E35" s="17" t="s">
         <v>98</v>
       </c>
@@ -3069,34 +3097,34 @@
       <c r="J35" s="17"/>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A36" s="70">
+      <c r="A36" s="55">
         <v>20</v>
       </c>
-      <c r="B36" s="38" t="s">
+      <c r="B36" s="32" t="s">
         <v>92</v>
       </c>
       <c r="C36" s="68"/>
-      <c r="D36" s="36"/>
-      <c r="E36" s="34" t="s">
+      <c r="D36" s="69"/>
+      <c r="E36" s="31" t="s">
         <v>99</v>
       </c>
-      <c r="F36" s="33"/>
-      <c r="G36" s="33"/>
+      <c r="F36" s="30"/>
+      <c r="G36" s="30"/>
       <c r="H36" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="I36" s="33"/>
-      <c r="J36" s="34"/>
-      <c r="K36" s="33"/>
+      <c r="I36" s="30"/>
+      <c r="J36" s="31"/>
+      <c r="K36" s="30"/>
     </row>
     <row r="37" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="70">
+      <c r="A37" s="55">
         <v>21</v>
       </c>
-      <c r="B37" s="39" t="s">
+      <c r="B37" s="33" t="s">
         <v>92</v>
       </c>
-      <c r="C37" s="67" t="s">
+      <c r="C37" s="54" t="s">
         <v>41</v>
       </c>
       <c r="D37" s="23"/>
@@ -3104,44 +3132,44 @@
       <c r="J37" s="17"/>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A38" s="70">
+      <c r="A38" s="55">
         <v>22</v>
       </c>
-      <c r="B38" s="38" t="s">
+      <c r="B38" s="32" t="s">
         <v>92</v>
       </c>
-      <c r="C38" s="66" t="s">
+      <c r="C38" s="53" t="s">
         <v>45</v>
       </c>
-      <c r="D38" s="31"/>
-      <c r="E38" s="34"/>
-      <c r="F38" s="33"/>
-      <c r="G38" s="33"/>
-      <c r="H38" s="33"/>
-      <c r="I38" s="33"/>
-      <c r="J38" s="34"/>
-      <c r="K38" s="33"/>
+      <c r="D38" s="28"/>
+      <c r="E38" s="31"/>
+      <c r="F38" s="30"/>
+      <c r="G38" s="30"/>
+      <c r="H38" s="30"/>
+      <c r="I38" s="30"/>
+      <c r="J38" s="31"/>
+      <c r="K38" s="30"/>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A39" s="70">
+      <c r="A39" s="55">
         <v>23</v>
       </c>
-      <c r="B39" s="38" t="s">
+      <c r="B39" s="32" t="s">
         <v>92</v>
       </c>
-      <c r="C39" s="66" t="s">
+      <c r="C39" s="53" t="s">
         <v>512</v>
       </c>
-      <c r="D39" s="31"/>
-      <c r="E39" s="34" t="s">
+      <c r="D39" s="28"/>
+      <c r="E39" s="31" t="s">
         <v>513</v>
       </c>
-      <c r="F39" s="33"/>
-      <c r="G39" s="33"/>
-      <c r="H39" s="33"/>
-      <c r="I39" s="33"/>
-      <c r="J39" s="34"/>
-      <c r="K39" s="33"/>
+      <c r="F39" s="30"/>
+      <c r="G39" s="30"/>
+      <c r="H39" s="30"/>
+      <c r="I39" s="30"/>
+      <c r="J39" s="31"/>
+      <c r="K39" s="30"/>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="E40" s="15" t="s">
@@ -3150,12 +3178,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A3:A9"/>
-    <mergeCell ref="A10:A15"/>
-    <mergeCell ref="A22:A26"/>
-    <mergeCell ref="B3:B9"/>
-    <mergeCell ref="B10:B15"/>
-    <mergeCell ref="B22:B26"/>
     <mergeCell ref="C35:C36"/>
     <mergeCell ref="D35:D36"/>
     <mergeCell ref="C3:C9"/>
@@ -3166,6 +3188,12 @@
     <mergeCell ref="D10:D15"/>
     <mergeCell ref="C22:C26"/>
     <mergeCell ref="D22:D26"/>
+    <mergeCell ref="A3:A9"/>
+    <mergeCell ref="A10:A15"/>
+    <mergeCell ref="A22:A26"/>
+    <mergeCell ref="B3:B9"/>
+    <mergeCell ref="B10:B15"/>
+    <mergeCell ref="B22:B26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3301,7 +3329,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="78" t="s">
         <v>22</v>
       </c>
       <c r="B2">
@@ -3309,61 +3337,61 @@
       </c>
     </row>
     <row r="3" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="29"/>
+      <c r="A3" s="78"/>
       <c r="B3">
         <v>457</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="29"/>
+      <c r="A4" s="78"/>
       <c r="B4">
         <v>473</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="29"/>
+      <c r="A5" s="78"/>
       <c r="B5">
         <v>491</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="29"/>
+      <c r="A6" s="78"/>
       <c r="B6">
         <v>514</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="29"/>
+      <c r="A7" s="78"/>
       <c r="B7">
         <v>532</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="29"/>
+      <c r="A8" s="78"/>
       <c r="B8">
         <v>561</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="29"/>
+      <c r="A9" s="78"/>
       <c r="B9">
         <v>640</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="29"/>
+      <c r="A10" s="78"/>
       <c r="B10">
         <v>660</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="29"/>
+      <c r="A11" s="78"/>
       <c r="B11">
         <v>780</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="29" t="s">
+      <c r="A12" s="78" t="s">
         <v>23</v>
       </c>
       <c r="B12">
@@ -3374,19 +3402,19 @@
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="29"/>
+      <c r="A13" s="78"/>
       <c r="B13">
         <v>830</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="29"/>
+      <c r="A14" s="78"/>
       <c r="B14">
         <v>980</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="29"/>
+      <c r="A15" s="78"/>
       <c r="B15">
         <v>1064</v>
       </c>

</xml_diff>

<commit_message>
added OEM, txt and JCAMP readers
</commit_message>
<xml_diff>
--- a/documents/Raman data formats.xlsx
+++ b/documents/Raman data formats.xlsx
@@ -9,15 +9,16 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="22152" windowHeight="10740"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="19308" windowHeight="6660" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="File formats" sheetId="6" r:id="rId1"/>
-    <sheet name="Test data" sheetId="5" r:id="rId2"/>
-    <sheet name="Models" sheetId="1" r:id="rId3"/>
-    <sheet name="Lasers" sheetId="4" r:id="rId4"/>
-    <sheet name="File formats table" sheetId="3" r:id="rId5"/>
-    <sheet name="Gwyddion" sheetId="7" r:id="rId6"/>
+    <sheet name="Tabelle1" sheetId="8" r:id="rId2"/>
+    <sheet name="Test data" sheetId="5" r:id="rId3"/>
+    <sheet name="Models" sheetId="1" r:id="rId4"/>
+    <sheet name="Lasers" sheetId="4" r:id="rId5"/>
+    <sheet name="File formats table" sheetId="3" r:id="rId6"/>
+    <sheet name="Gwyddion" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1278" uniqueCount="519">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1326" uniqueCount="541">
   <si>
     <t>Renishaw InVia</t>
   </si>
@@ -1561,9 +1562,6 @@
     <t>specio, https://specio.readthedocs.io</t>
   </si>
   <si>
-    <t>OPUSFC, https://github.com/stuart-cls/python-opusfc-dist</t>
-  </si>
-  <si>
     <t>".0"</t>
   </si>
   <si>
@@ -1589,6 +1587,75 @@
   </si>
   <si>
     <t>t.b.d.</t>
+  </si>
+  <si>
+    <t>WXD (wire &lt;4.x)</t>
+  </si>
+  <si>
+    <t>Spectragryph can open</t>
+  </si>
+  <si>
+    <t>WXD is outdated since Wire 4.X (2015). Could not find file format description. Spectragryph can't open those either.</t>
+  </si>
+  <si>
+    <t>Spectragryph can't open those either.</t>
+  </si>
+  <si>
+    <t>OPUSFC, https://github.com/stuart-cls/python-opusfc-dist; spectrochempy</t>
+  </si>
+  <si>
+    <t>various</t>
+  </si>
+  <si>
+    <t>JCAMP-DX</t>
+  </si>
+  <si>
+    <t>.jdx, .dx</t>
+  </si>
+  <si>
+    <t>CSV</t>
+  </si>
+  <si>
+    <t>Format</t>
+  </si>
+  <si>
+    <t>Manufacturer</t>
+  </si>
+  <si>
+    <t>extensions</t>
+  </si>
+  <si>
+    <t>Text</t>
+  </si>
+  <si>
+    <t>various (BWTec, Ostec, RRUFF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPC </t>
+  </si>
+  <si>
+    <t>various (Galactic Industries)</t>
+  </si>
+  <si>
+    <t>SPA</t>
+  </si>
+  <si>
+    <t>.spa</t>
+  </si>
+  <si>
+    <t>Thermo Fisher / Nicolet</t>
+  </si>
+  <si>
+    <t>WDF</t>
+  </si>
+  <si>
+    <t>Renishaw Wire &gt;4.X</t>
+  </si>
+  <si>
+    <t>.txt, .txtr, .prn, …</t>
+  </si>
+  <si>
+    <t>.0, .1, …</t>
   </si>
 </sst>
 </file>
@@ -1737,15 +1804,13 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <i/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1856,7 +1921,7 @@
     <xf numFmtId="0" fontId="17" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="96">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2016,6 +2081,45 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="1" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="1" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="0" xfId="7" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -2025,12 +2129,18 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -2043,6 +2153,12 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="3" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="4" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2064,45 +2180,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="1" xfId="7" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="1" xfId="6" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="6" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="0" xfId="7" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="3" xfId="6" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="4" xfId="6" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="0" xfId="7" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="6" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="Gut" xfId="4" builtinId="26"/>
@@ -2482,20 +2569,21 @@
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="A1:K40"/>
+  <dimension ref="A1:K42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+    <sheetView topLeftCell="A10" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="6.5546875" style="14" customWidth="1"/>
-    <col min="3" max="3" width="20.77734375" customWidth="1"/>
-    <col min="5" max="5" width="27.5546875" style="1" customWidth="1"/>
+    <col min="1" max="2" width="5.109375" style="14" customWidth="1"/>
+    <col min="3" max="3" width="14.109375" customWidth="1"/>
+    <col min="4" max="4" width="10.44140625" customWidth="1"/>
+    <col min="5" max="5" width="25.5546875" style="1" customWidth="1"/>
     <col min="6" max="6" width="10" customWidth="1"/>
-    <col min="7" max="7" width="39.44140625" customWidth="1"/>
-    <col min="10" max="10" width="59.77734375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="26.5546875" customWidth="1"/>
+    <col min="10" max="10" width="49.109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="5" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -2530,27 +2618,23 @@
         <v>93</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="16" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A2" s="33">
-        <v>1</v>
-      </c>
-      <c r="B2" s="21" t="s">
+    <row r="2" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="66"/>
+      <c r="B2" s="67" t="s">
         <v>90</v>
       </c>
-      <c r="C2" s="43" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" s="22" t="s">
-        <v>27</v>
-      </c>
+      <c r="C2" s="68" t="s">
+        <v>526</v>
+      </c>
+      <c r="D2" s="69"/>
       <c r="E2" s="34" t="s">
-        <v>94</v>
+        <v>112</v>
       </c>
       <c r="F2" s="54" t="s">
         <v>60</v>
       </c>
       <c r="G2" s="55" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="H2" s="54" t="s">
         <v>60</v>
@@ -2558,637 +2642,669 @@
       <c r="I2" s="54" t="s">
         <v>60</v>
       </c>
-      <c r="J2" s="36" t="s">
+      <c r="J2" s="36"/>
+    </row>
+    <row r="3" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="66"/>
+      <c r="B3" s="67" t="s">
+        <v>90</v>
+      </c>
+      <c r="C3" s="68" t="s">
+        <v>524</v>
+      </c>
+      <c r="D3" s="69"/>
+      <c r="E3" s="34" t="s">
+        <v>525</v>
+      </c>
+      <c r="F3" s="54" t="s">
+        <v>60</v>
+      </c>
+      <c r="G3" s="55" t="s">
+        <v>515</v>
+      </c>
+      <c r="H3" s="54" t="s">
+        <v>60</v>
+      </c>
+      <c r="I3" s="54" t="s">
+        <v>60</v>
+      </c>
+      <c r="J3" s="36"/>
+    </row>
+    <row r="4" spans="1:11" s="16" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A4" s="33">
+        <v>1</v>
+      </c>
+      <c r="B4" s="21" t="s">
+        <v>90</v>
+      </c>
+      <c r="C4" s="43" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" s="34" t="s">
+        <v>94</v>
+      </c>
+      <c r="F4" s="54" t="s">
+        <v>60</v>
+      </c>
+      <c r="G4" s="55" t="s">
+        <v>515</v>
+      </c>
+      <c r="H4" s="54" t="s">
+        <v>60</v>
+      </c>
+      <c r="I4" s="54" t="s">
+        <v>60</v>
+      </c>
+      <c r="J4" s="36" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="3" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="68">
+    <row r="5" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="85">
         <v>2</v>
       </c>
-      <c r="B3" s="71" t="s">
+      <c r="B5" s="88" t="s">
         <v>90</v>
       </c>
-      <c r="C3" s="61" t="s">
+      <c r="C5" s="74" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="78" t="s">
+      <c r="D5" s="75" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="85" t="s">
+      <c r="E5" s="78" t="s">
         <v>69</v>
       </c>
-      <c r="F3" s="62" t="s">
+      <c r="F5" s="76" t="s">
         <v>60</v>
       </c>
-      <c r="G3" s="56"/>
-      <c r="H3" s="83" t="s">
-        <v>517</v>
-      </c>
-      <c r="I3" s="83" t="s">
-        <v>517</v>
-      </c>
-      <c r="J3" s="37"/>
-      <c r="K3" s="29"/>
-    </row>
-    <row r="4" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="68"/>
-      <c r="B4" s="71"/>
-      <c r="C4" s="61"/>
-      <c r="D4" s="78"/>
-      <c r="E4" s="85"/>
-      <c r="F4" s="63"/>
-      <c r="G4" s="56"/>
-      <c r="H4" s="84"/>
-      <c r="I4" s="84"/>
-      <c r="J4" s="37"/>
-      <c r="K4" s="29"/>
-    </row>
-    <row r="5" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="68"/>
-      <c r="B5" s="71"/>
-      <c r="C5" s="61"/>
-      <c r="D5" s="78"/>
-      <c r="E5" s="38" t="s">
-        <v>70</v>
-      </c>
-      <c r="F5" s="53" t="s">
-        <v>60</v>
-      </c>
-      <c r="G5" s="56" t="s">
-        <v>515</v>
-      </c>
-      <c r="H5" s="53" t="s">
-        <v>60</v>
-      </c>
-      <c r="I5" s="53" t="s">
-        <v>60</v>
+      <c r="G5" s="56"/>
+      <c r="H5" s="83" t="s">
+        <v>516</v>
+      </c>
+      <c r="I5" s="83" t="s">
+        <v>516</v>
       </c>
       <c r="J5" s="37"/>
       <c r="K5" s="29"/>
     </row>
     <row r="6" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="68"/>
-      <c r="B6" s="71"/>
-      <c r="C6" s="61"/>
-      <c r="D6" s="78"/>
-      <c r="E6" s="86" t="s">
-        <v>71</v>
-      </c>
-      <c r="F6" s="53" t="s">
-        <v>60</v>
-      </c>
+      <c r="A6" s="85"/>
+      <c r="B6" s="88"/>
+      <c r="C6" s="74"/>
+      <c r="D6" s="75"/>
+      <c r="E6" s="78"/>
+      <c r="F6" s="77"/>
       <c r="G6" s="56"/>
-      <c r="H6" s="76" t="s">
-        <v>517</v>
-      </c>
-      <c r="I6" s="76" t="s">
-        <v>517</v>
-      </c>
+      <c r="H6" s="84"/>
+      <c r="I6" s="84"/>
       <c r="J6" s="37"/>
       <c r="K6" s="29"/>
     </row>
     <row r="7" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="68"/>
-      <c r="B7" s="71"/>
-      <c r="C7" s="61"/>
-      <c r="D7" s="78"/>
-      <c r="E7" s="86" t="s">
-        <v>72</v>
-      </c>
-      <c r="F7" s="56"/>
-      <c r="G7" s="56"/>
-      <c r="H7" s="76" t="s">
-        <v>517</v>
-      </c>
-      <c r="I7" s="76" t="s">
-        <v>517</v>
+      <c r="A7" s="85"/>
+      <c r="B7" s="88"/>
+      <c r="C7" s="74"/>
+      <c r="D7" s="75"/>
+      <c r="E7" s="38" t="s">
+        <v>70</v>
+      </c>
+      <c r="F7" s="53" t="s">
+        <v>60</v>
+      </c>
+      <c r="G7" s="56" t="s">
+        <v>514</v>
+      </c>
+      <c r="H7" s="53" t="s">
+        <v>60</v>
+      </c>
+      <c r="I7" s="53" t="s">
+        <v>60</v>
       </c>
       <c r="J7" s="37"/>
       <c r="K7" s="29"/>
     </row>
-    <row r="8" spans="1:11" s="16" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A8" s="68"/>
-      <c r="B8" s="71"/>
-      <c r="C8" s="61"/>
-      <c r="D8" s="78"/>
-      <c r="E8" s="38" t="s">
-        <v>97</v>
+    <row r="8" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="85"/>
+      <c r="B8" s="88"/>
+      <c r="C8" s="74"/>
+      <c r="D8" s="75"/>
+      <c r="E8" s="64" t="s">
+        <v>71</v>
       </c>
       <c r="F8" s="53" t="s">
         <v>60</v>
       </c>
-      <c r="G8" s="57" t="s">
-        <v>506</v>
-      </c>
-      <c r="H8" s="53" t="s">
-        <v>60</v>
-      </c>
-      <c r="I8" s="53" t="s">
-        <v>60</v>
-      </c>
-      <c r="J8" s="39"/>
+      <c r="G8" s="56"/>
+      <c r="H8" s="60" t="s">
+        <v>516</v>
+      </c>
+      <c r="I8" s="60" t="s">
+        <v>516</v>
+      </c>
+      <c r="J8" s="37"/>
       <c r="K8" s="29"/>
     </row>
     <row r="9" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="68"/>
-      <c r="B9" s="71"/>
-      <c r="C9" s="61"/>
-      <c r="D9" s="78"/>
-      <c r="E9" s="77" t="s">
-        <v>73</v>
-      </c>
-      <c r="F9" s="76" t="s">
-        <v>518</v>
-      </c>
+      <c r="A9" s="85"/>
+      <c r="B9" s="88"/>
+      <c r="C9" s="74"/>
+      <c r="D9" s="75"/>
+      <c r="E9" s="64" t="s">
+        <v>72</v>
+      </c>
+      <c r="F9" s="56"/>
       <c r="G9" s="56"/>
-      <c r="H9" s="75" t="s">
-        <v>517</v>
-      </c>
-      <c r="I9" s="75" t="s">
-        <v>517</v>
+      <c r="H9" s="60" t="s">
+        <v>516</v>
+      </c>
+      <c r="I9" s="60" t="s">
+        <v>516</v>
       </c>
       <c r="J9" s="37"/>
       <c r="K9" s="29"/>
     </row>
-    <row r="10" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="69">
-        <v>3</v>
-      </c>
-      <c r="B10" s="72" t="s">
-        <v>90</v>
-      </c>
-      <c r="C10" s="64" t="s">
-        <v>15</v>
-      </c>
-      <c r="D10" s="65" t="s">
-        <v>28</v>
-      </c>
-      <c r="E10" s="80" t="s">
-        <v>82</v>
-      </c>
-      <c r="F10" s="76" t="s">
-        <v>518</v>
-      </c>
-      <c r="G10" s="58"/>
+    <row r="10" spans="1:11" s="16" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A10" s="85"/>
+      <c r="B10" s="88"/>
+      <c r="C10" s="74"/>
+      <c r="D10" s="75"/>
+      <c r="E10" s="38" t="s">
+        <v>97</v>
+      </c>
+      <c r="F10" s="53" t="s">
+        <v>60</v>
+      </c>
+      <c r="G10" s="57" t="s">
+        <v>506</v>
+      </c>
       <c r="H10" s="53" t="s">
         <v>60</v>
       </c>
-      <c r="I10" s="76" t="s">
-        <v>517</v>
-      </c>
-      <c r="J10" s="36"/>
+      <c r="I10" s="53" t="s">
+        <v>60</v>
+      </c>
+      <c r="J10" s="39"/>
+      <c r="K10" s="29"/>
     </row>
     <row r="11" spans="1:11" s="16" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A11" s="69"/>
-      <c r="B11" s="72"/>
-      <c r="C11" s="64"/>
-      <c r="D11" s="65"/>
-      <c r="E11" s="79" t="s">
+      <c r="A11" s="85"/>
+      <c r="B11" s="88"/>
+      <c r="C11" s="74"/>
+      <c r="D11" s="75"/>
+      <c r="E11" s="64" t="s">
+        <v>518</v>
+      </c>
+      <c r="F11" s="65" t="s">
+        <v>516</v>
+      </c>
+      <c r="G11" s="56"/>
+      <c r="H11" s="53" t="s">
+        <v>60</v>
+      </c>
+      <c r="I11" s="59" t="s">
+        <v>516</v>
+      </c>
+      <c r="J11" s="93" t="s">
+        <v>520</v>
+      </c>
+      <c r="K11" s="29"/>
+    </row>
+    <row r="12" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="86">
+        <v>3</v>
+      </c>
+      <c r="B12" s="89" t="s">
+        <v>90</v>
+      </c>
+      <c r="C12" s="79" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" s="80" t="s">
+        <v>28</v>
+      </c>
+      <c r="E12" s="62" t="s">
+        <v>82</v>
+      </c>
+      <c r="F12" s="53" t="s">
+        <v>60</v>
+      </c>
+      <c r="G12" s="58" t="s">
+        <v>515</v>
+      </c>
+      <c r="H12" s="53" t="s">
+        <v>60</v>
+      </c>
+      <c r="I12" s="53" t="s">
+        <v>60</v>
+      </c>
+      <c r="J12" s="36"/>
+    </row>
+    <row r="13" spans="1:11" s="16" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="86"/>
+      <c r="B13" s="89"/>
+      <c r="C13" s="79"/>
+      <c r="D13" s="80"/>
+      <c r="E13" s="62" t="s">
         <v>77</v>
       </c>
-      <c r="F11" s="76" t="s">
-        <v>518</v>
-      </c>
-      <c r="G11" s="58"/>
-      <c r="H11" s="75" t="s">
-        <v>517</v>
-      </c>
-      <c r="I11" s="75" t="s">
-        <v>517</v>
-      </c>
-      <c r="J11" s="36"/>
-    </row>
-    <row r="12" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="69"/>
-      <c r="B12" s="72"/>
-      <c r="C12" s="64"/>
-      <c r="D12" s="65"/>
-      <c r="E12" s="79" t="s">
+      <c r="F13" s="65" t="s">
+        <v>516</v>
+      </c>
+      <c r="G13" s="58"/>
+      <c r="H13" s="53" t="s">
+        <v>60</v>
+      </c>
+      <c r="I13" s="59" t="s">
+        <v>516</v>
+      </c>
+      <c r="J13" s="92" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="86"/>
+      <c r="B14" s="89"/>
+      <c r="C14" s="79"/>
+      <c r="D14" s="80"/>
+      <c r="E14" s="62" t="s">
         <v>78</v>
       </c>
-      <c r="F12" s="76" t="s">
-        <v>518</v>
-      </c>
-      <c r="G12" s="58"/>
-      <c r="H12" s="75" t="s">
-        <v>517</v>
-      </c>
-      <c r="I12" s="75" t="s">
-        <v>517</v>
-      </c>
-      <c r="J12" s="36"/>
-    </row>
-    <row r="13" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="69"/>
-      <c r="B13" s="72"/>
-      <c r="C13" s="64"/>
-      <c r="D13" s="65"/>
-      <c r="E13" s="79" t="s">
-        <v>79</v>
-      </c>
-      <c r="F13" s="76" t="s">
-        <v>518</v>
-      </c>
-      <c r="G13" s="58"/>
-      <c r="H13" s="75" t="s">
-        <v>517</v>
-      </c>
-      <c r="I13" s="75" t="s">
-        <v>517</v>
-      </c>
-      <c r="J13" s="36"/>
-    </row>
-    <row r="14" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="69"/>
-      <c r="B14" s="72"/>
-      <c r="C14" s="64"/>
-      <c r="D14" s="65"/>
-      <c r="E14" s="80" t="s">
-        <v>80</v>
-      </c>
-      <c r="F14" s="53" t="s">
-        <v>60</v>
-      </c>
-      <c r="G14" s="56" t="s">
-        <v>515</v>
-      </c>
+      <c r="F14" s="65" t="s">
+        <v>516</v>
+      </c>
+      <c r="G14" s="58"/>
       <c r="H14" s="53" t="s">
         <v>60</v>
       </c>
-      <c r="I14" s="76" t="s">
-        <v>517</v>
-      </c>
-      <c r="J14" s="36"/>
+      <c r="I14" s="59" t="s">
+        <v>516</v>
+      </c>
+      <c r="J14" s="92" t="s">
+        <v>519</v>
+      </c>
     </row>
     <row r="15" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="69"/>
-      <c r="B15" s="72"/>
-      <c r="C15" s="64"/>
-      <c r="D15" s="65"/>
-      <c r="E15" s="40" t="s">
-        <v>81</v>
-      </c>
-      <c r="F15" s="53" t="s">
+      <c r="A15" s="86"/>
+      <c r="B15" s="89"/>
+      <c r="C15" s="79"/>
+      <c r="D15" s="80"/>
+      <c r="E15" s="61" t="s">
+        <v>79</v>
+      </c>
+      <c r="F15" s="94" t="s">
+        <v>516</v>
+      </c>
+      <c r="G15" s="58"/>
+      <c r="H15" s="60" t="s">
+        <v>516</v>
+      </c>
+      <c r="I15" s="60" t="s">
+        <v>516</v>
+      </c>
+      <c r="J15" s="36"/>
+    </row>
+    <row r="16" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="86"/>
+      <c r="B16" s="89"/>
+      <c r="C16" s="79"/>
+      <c r="D16" s="80"/>
+      <c r="E16" s="62" t="s">
+        <v>80</v>
+      </c>
+      <c r="F16" s="53" t="s">
         <v>60</v>
       </c>
-      <c r="G15" s="55" t="s">
-        <v>516</v>
-      </c>
-      <c r="H15" s="53" t="s">
-        <v>60</v>
-      </c>
-      <c r="I15" s="53" t="s">
-        <v>60</v>
-      </c>
-      <c r="J15" s="36"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A16" s="41">
-        <v>4</v>
-      </c>
-      <c r="B16" s="26" t="s">
-        <v>90</v>
-      </c>
-      <c r="C16" s="44" t="s">
-        <v>16</v>
-      </c>
-      <c r="D16" s="27" t="s">
-        <v>25</v>
-      </c>
-      <c r="E16" s="42" t="s">
-        <v>96</v>
-      </c>
-      <c r="F16" s="87" t="s">
-        <v>517</v>
-      </c>
-      <c r="G16" s="30" t="s">
-        <v>31</v>
+      <c r="G16" s="56" t="s">
+        <v>514</v>
       </c>
       <c r="H16" s="53" t="s">
         <v>60</v>
       </c>
-      <c r="I16" s="76" t="s">
-        <v>517</v>
-      </c>
-      <c r="J16" s="37" t="s">
-        <v>514</v>
-      </c>
-      <c r="K16" s="29"/>
+      <c r="I16" s="53" t="s">
+        <v>60</v>
+      </c>
+      <c r="J16" s="36"/>
     </row>
     <row r="17" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="41">
-        <v>5</v>
-      </c>
-      <c r="B17" s="21" t="s">
-        <v>90</v>
-      </c>
-      <c r="C17" s="43" t="s">
-        <v>18</v>
-      </c>
-      <c r="D17" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="E17" s="81" t="s">
-        <v>33</v>
-      </c>
-      <c r="F17" s="76" t="s">
-        <v>518</v>
-      </c>
-      <c r="G17" s="35"/>
-      <c r="H17" s="87" t="s">
-        <v>517</v>
-      </c>
-      <c r="I17" s="75" t="s">
-        <v>517</v>
+      <c r="A17" s="86"/>
+      <c r="B17" s="89"/>
+      <c r="C17" s="79"/>
+      <c r="D17" s="80"/>
+      <c r="E17" s="40" t="s">
+        <v>81</v>
+      </c>
+      <c r="F17" s="53" t="s">
+        <v>60</v>
+      </c>
+      <c r="G17" s="55" t="s">
+        <v>515</v>
+      </c>
+      <c r="H17" s="53" t="s">
+        <v>60</v>
+      </c>
+      <c r="I17" s="53" t="s">
+        <v>60</v>
       </c>
       <c r="J17" s="36"/>
     </row>
-    <row r="18" spans="1:11" s="16" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="41">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B18" s="26" t="s">
         <v>90</v>
       </c>
       <c r="C18" s="44" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D18" s="27" t="s">
-        <v>40</v>
-      </c>
-      <c r="E18" s="82" t="s">
-        <v>510</v>
-      </c>
-      <c r="F18" s="53" t="s">
+        <v>25</v>
+      </c>
+      <c r="E18" s="42" t="s">
+        <v>96</v>
+      </c>
+      <c r="F18" s="65" t="s">
+        <v>516</v>
+      </c>
+      <c r="G18" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="H18" s="53" t="s">
         <v>60</v>
       </c>
-      <c r="G18" s="37" t="s">
-        <v>509</v>
-      </c>
-      <c r="H18" s="87" t="s">
-        <v>517</v>
-      </c>
-      <c r="I18" s="75" t="s">
-        <v>517</v>
-      </c>
-      <c r="J18" s="37"/>
+      <c r="I18" s="60" t="s">
+        <v>516</v>
+      </c>
+      <c r="J18" s="37" t="s">
+        <v>513</v>
+      </c>
       <c r="K18" s="29"/>
     </row>
     <row r="19" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="41">
+        <v>5</v>
+      </c>
+      <c r="B19" s="21" t="s">
+        <v>90</v>
+      </c>
+      <c r="C19" s="43" t="s">
+        <v>18</v>
+      </c>
+      <c r="D19" s="71" t="s">
+        <v>32</v>
+      </c>
+      <c r="E19" s="63" t="s">
+        <v>33</v>
+      </c>
+      <c r="F19" s="60" t="s">
+        <v>517</v>
+      </c>
+      <c r="G19" s="35"/>
+      <c r="H19" s="65" t="s">
+        <v>516</v>
+      </c>
+      <c r="I19" s="59" t="s">
+        <v>516</v>
+      </c>
+      <c r="J19" s="93" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" s="16" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A20" s="41">
+        <v>6</v>
+      </c>
+      <c r="B20" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="C20" s="44" t="s">
+        <v>19</v>
+      </c>
+      <c r="D20" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="E20" s="70" t="s">
+        <v>509</v>
+      </c>
+      <c r="F20" s="53" t="s">
+        <v>60</v>
+      </c>
+      <c r="G20" s="37" t="s">
+        <v>522</v>
+      </c>
+      <c r="H20" s="53" t="s">
+        <v>60</v>
+      </c>
+      <c r="I20" s="53" t="s">
+        <v>60</v>
+      </c>
+      <c r="J20" s="37"/>
+      <c r="K20" s="29"/>
+    </row>
+    <row r="21" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="41">
         <v>8</v>
       </c>
-      <c r="B19" s="26" t="s">
+      <c r="B21" s="26" t="s">
         <v>90</v>
       </c>
-      <c r="C19" s="44" t="s">
+      <c r="C21" s="44" t="s">
         <v>17</v>
       </c>
-      <c r="D19" s="27" t="s">
+      <c r="D21" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="E19" s="28" t="s">
+      <c r="E21" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="F19" s="53" t="s">
+      <c r="F21" s="53" t="s">
         <v>60</v>
       </c>
-      <c r="G19" s="30" t="s">
+      <c r="G21" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="H19" s="53" t="s">
+      <c r="H21" s="53" t="s">
         <v>60</v>
       </c>
-      <c r="I19" s="53" t="s">
+      <c r="I21" s="53" t="s">
         <v>60</v>
       </c>
-      <c r="J19" s="30"/>
-      <c r="K19" s="29"/>
-    </row>
-    <row r="20" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="41">
-        <v>9</v>
-      </c>
-      <c r="B20" s="47" t="s">
-        <v>91</v>
-      </c>
-      <c r="C20" s="48" t="s">
-        <v>61</v>
-      </c>
-      <c r="D20" s="22" t="s">
-        <v>62</v>
-      </c>
-      <c r="E20" s="20" t="s">
-        <v>62</v>
-      </c>
-      <c r="J20" s="17"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A21" s="41">
-        <v>10</v>
-      </c>
-      <c r="B21" s="45" t="s">
-        <v>91</v>
-      </c>
-      <c r="C21" s="46" t="s">
-        <v>36</v>
-      </c>
-      <c r="D21" s="27"/>
-      <c r="E21" s="28" t="s">
-        <v>37</v>
-      </c>
-      <c r="F21" s="29"/>
-      <c r="G21" s="29"/>
-      <c r="H21" s="29"/>
-      <c r="I21" s="29"/>
       <c r="J21" s="30"/>
       <c r="K21" s="29"/>
     </row>
     <row r="22" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="70">
+      <c r="A22" s="41">
+        <v>9</v>
+      </c>
+      <c r="B22" s="47" t="s">
+        <v>91</v>
+      </c>
+      <c r="C22" s="48" t="s">
+        <v>61</v>
+      </c>
+      <c r="D22" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="E22" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="J22" s="17"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A23" s="41">
+        <v>10</v>
+      </c>
+      <c r="B23" s="45" t="s">
+        <v>91</v>
+      </c>
+      <c r="C23" s="46" t="s">
+        <v>36</v>
+      </c>
+      <c r="D23" s="27"/>
+      <c r="E23" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="F23" s="29"/>
+      <c r="G23" s="29"/>
+      <c r="H23" s="29"/>
+      <c r="I23" s="29"/>
+      <c r="J23" s="30"/>
+      <c r="K23" s="29"/>
+    </row>
+    <row r="24" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="87">
         <v>11</v>
       </c>
-      <c r="B22" s="73" t="s">
+      <c r="B24" s="90" t="s">
         <v>91</v>
       </c>
-      <c r="C22" s="66" t="s">
+      <c r="C24" s="81" t="s">
         <v>64</v>
       </c>
-      <c r="D22" s="67"/>
-      <c r="E22" s="17" t="s">
+      <c r="D24" s="82"/>
+      <c r="E24" s="17" t="s">
         <v>88</v>
       </c>
-      <c r="J22" s="17"/>
-    </row>
-    <row r="23" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="70"/>
-      <c r="B23" s="73"/>
-      <c r="C23" s="66"/>
-      <c r="D23" s="67"/>
-      <c r="E23" s="17" t="s">
+      <c r="F24" s="53" t="s">
+        <v>60</v>
+      </c>
+      <c r="J24" s="17"/>
+    </row>
+    <row r="25" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="87"/>
+      <c r="B25" s="90"/>
+      <c r="C25" s="81"/>
+      <c r="D25" s="82"/>
+      <c r="E25" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="J23" s="17"/>
-    </row>
-    <row r="24" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="70"/>
-      <c r="B24" s="73"/>
-      <c r="C24" s="66"/>
-      <c r="D24" s="67"/>
-      <c r="E24" s="17" t="s">
+      <c r="J25" s="17"/>
+    </row>
+    <row r="26" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="87"/>
+      <c r="B26" s="90"/>
+      <c r="C26" s="81"/>
+      <c r="D26" s="82"/>
+      <c r="E26" s="17" t="s">
         <v>85</v>
       </c>
-      <c r="J24" s="17"/>
-    </row>
-    <row r="25" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="70"/>
-      <c r="B25" s="73"/>
-      <c r="C25" s="66"/>
-      <c r="D25" s="67"/>
-      <c r="E25" s="17" t="s">
+      <c r="J26" s="17"/>
+    </row>
+    <row r="27" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="87"/>
+      <c r="B27" s="90"/>
+      <c r="C27" s="81"/>
+      <c r="D27" s="82"/>
+      <c r="E27" s="17" t="s">
         <v>86</v>
       </c>
-      <c r="J25" s="17"/>
-    </row>
-    <row r="26" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="70"/>
-      <c r="B26" s="73"/>
-      <c r="C26" s="66"/>
-      <c r="D26" s="67"/>
-      <c r="E26" s="17" t="s">
+      <c r="J27" s="17"/>
+    </row>
+    <row r="28" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="87"/>
+      <c r="B28" s="90"/>
+      <c r="C28" s="81"/>
+      <c r="D28" s="82"/>
+      <c r="E28" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="J26" s="17"/>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A27" s="52">
+      <c r="J28" s="17"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A29" s="52">
         <v>12</v>
       </c>
-      <c r="B27" s="45" t="s">
+      <c r="B29" s="45" t="s">
         <v>91</v>
       </c>
-      <c r="C27" s="46" t="s">
+      <c r="C29" s="46" t="s">
         <v>46</v>
       </c>
-      <c r="D27" s="27"/>
-      <c r="E27" s="30"/>
-      <c r="F27" s="29"/>
-      <c r="G27" s="29"/>
-      <c r="H27" s="29"/>
-      <c r="I27" s="29"/>
-      <c r="J27" s="30"/>
-      <c r="K27" s="29"/>
-    </row>
-    <row r="28" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="52">
-        <v>13</v>
-      </c>
-      <c r="B28" s="47" t="s">
-        <v>91</v>
-      </c>
-      <c r="C28" s="48" t="s">
-        <v>57</v>
-      </c>
-      <c r="D28" s="22" t="s">
-        <v>58</v>
-      </c>
-      <c r="E28" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="G28" s="55" t="s">
-        <v>516</v>
-      </c>
-      <c r="H28" s="19" t="s">
-        <v>60</v>
-      </c>
-      <c r="I28" s="19" t="s">
-        <v>60</v>
-      </c>
-      <c r="J28" s="17"/>
-    </row>
-    <row r="29" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="41">
-        <v>7</v>
-      </c>
-      <c r="B29" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="C29" s="49" t="s">
-        <v>55</v>
-      </c>
-      <c r="D29" s="22" t="s">
-        <v>56</v>
-      </c>
-      <c r="E29" s="34" t="s">
-        <v>66</v>
-      </c>
-      <c r="F29" s="19" t="s">
-        <v>60</v>
-      </c>
-      <c r="G29" s="36" t="s">
-        <v>508</v>
-      </c>
-      <c r="H29" s="19" t="s">
-        <v>60</v>
-      </c>
-      <c r="I29" s="35" t="s">
-        <v>511</v>
-      </c>
-      <c r="J29" s="36"/>
+      <c r="D29" s="27"/>
+      <c r="E29" s="30"/>
+      <c r="F29" s="29"/>
+      <c r="G29" s="29"/>
+      <c r="H29" s="29"/>
+      <c r="I29" s="29"/>
+      <c r="J29" s="30"/>
+      <c r="K29" s="29"/>
     </row>
     <row r="30" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="52">
-        <v>14</v>
-      </c>
-      <c r="B30" s="31" t="s">
-        <v>92</v>
-      </c>
-      <c r="C30" s="50" t="s">
-        <v>47</v>
-      </c>
-      <c r="D30" s="27"/>
-      <c r="E30" s="28"/>
-      <c r="F30" s="29"/>
-      <c r="G30" s="29"/>
-      <c r="H30" s="29"/>
-      <c r="I30" s="29"/>
-      <c r="J30" s="30"/>
-      <c r="K30" s="29"/>
+        <v>13</v>
+      </c>
+      <c r="B30" s="47" t="s">
+        <v>91</v>
+      </c>
+      <c r="C30" s="48" t="s">
+        <v>57</v>
+      </c>
+      <c r="D30" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="E30" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="F30" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="G30" s="55" t="s">
+        <v>515</v>
+      </c>
+      <c r="H30" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="I30" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="J30" s="17"/>
     </row>
     <row r="31" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="52">
-        <v>15</v>
-      </c>
-      <c r="B31" s="32" t="s">
-        <v>92</v>
-      </c>
-      <c r="C31" s="51" t="s">
-        <v>34</v>
-      </c>
-      <c r="D31" s="22"/>
-      <c r="E31" s="20" t="s">
-        <v>35</v>
+      <c r="A31" s="41">
+        <v>7</v>
+      </c>
+      <c r="B31" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="C31" s="49" t="s">
+        <v>55</v>
+      </c>
+      <c r="D31" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="E31" s="34" t="s">
+        <v>66</v>
       </c>
       <c r="F31" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="J31" s="17"/>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="G31" s="36" t="s">
+        <v>508</v>
+      </c>
+      <c r="H31" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="I31" s="35" t="s">
+        <v>510</v>
+      </c>
+      <c r="J31" s="36"/>
+    </row>
+    <row r="32" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A32" s="52">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B32" s="31" t="s">
         <v>92</v>
       </c>
       <c r="C32" s="50" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="D32" s="27"/>
-      <c r="E32" s="28" t="s">
-        <v>39</v>
-      </c>
+      <c r="E32" s="28"/>
       <c r="F32" s="29"/>
       <c r="G32" s="29"/>
       <c r="H32" s="29"/>
@@ -3198,33 +3314,40 @@
     </row>
     <row r="33" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A33" s="52">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B33" s="32" t="s">
         <v>92</v>
       </c>
       <c r="C33" s="51" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="D33" s="22"/>
       <c r="E33" s="20" t="s">
-        <v>63</v>
+        <v>35</v>
+      </c>
+      <c r="F33" s="19" t="s">
+        <v>60</v>
       </c>
       <c r="J33" s="17"/>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" s="52">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B34" s="31" t="s">
         <v>92</v>
       </c>
       <c r="C34" s="50" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="D34" s="27"/>
-      <c r="E34" s="30"/>
-      <c r="F34" s="29"/>
+      <c r="E34" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="F34" s="19" t="s">
+        <v>60</v>
+      </c>
       <c r="G34" s="29"/>
       <c r="H34" s="29"/>
       <c r="I34" s="29"/>
@@ -3233,125 +3356,165 @@
     </row>
     <row r="35" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A35" s="52">
-        <v>19</v>
-      </c>
-      <c r="B35" s="32"/>
-      <c r="C35" s="59" t="s">
-        <v>44</v>
-      </c>
-      <c r="D35" s="60"/>
-      <c r="E35" s="17" t="s">
-        <v>98</v>
-      </c>
-      <c r="H35" s="19" t="s">
-        <v>60</v>
+        <v>17</v>
+      </c>
+      <c r="B35" s="32" t="s">
+        <v>92</v>
+      </c>
+      <c r="C35" s="51" t="s">
+        <v>42</v>
+      </c>
+      <c r="D35" s="22"/>
+      <c r="E35" s="20" t="s">
+        <v>63</v>
       </c>
       <c r="J35" s="17"/>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36" s="52">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B36" s="31" t="s">
         <v>92</v>
       </c>
-      <c r="C36" s="59"/>
-      <c r="D36" s="60"/>
-      <c r="E36" s="30" t="s">
-        <v>99</v>
-      </c>
+      <c r="C36" s="50" t="s">
+        <v>43</v>
+      </c>
+      <c r="D36" s="27"/>
+      <c r="E36" s="30"/>
       <c r="F36" s="29"/>
       <c r="G36" s="29"/>
-      <c r="H36" s="19" t="s">
-        <v>60</v>
-      </c>
+      <c r="H36" s="29"/>
       <c r="I36" s="29"/>
       <c r="J36" s="30"/>
       <c r="K36" s="29"/>
     </row>
     <row r="37" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37" s="52">
-        <v>21</v>
-      </c>
-      <c r="B37" s="32" t="s">
-        <v>92</v>
-      </c>
-      <c r="C37" s="51" t="s">
-        <v>41</v>
-      </c>
-      <c r="D37" s="22"/>
-      <c r="E37" s="17"/>
+        <v>19</v>
+      </c>
+      <c r="B37" s="32"/>
+      <c r="C37" s="72" t="s">
+        <v>44</v>
+      </c>
+      <c r="D37" s="73"/>
+      <c r="E37" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="F37" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="H37" s="19" t="s">
+        <v>60</v>
+      </c>
       <c r="J37" s="17"/>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38" s="52">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B38" s="31" t="s">
         <v>92</v>
       </c>
-      <c r="C38" s="50" t="s">
-        <v>45</v>
-      </c>
-      <c r="D38" s="27"/>
-      <c r="E38" s="30"/>
-      <c r="F38" s="29"/>
+      <c r="C38" s="72"/>
+      <c r="D38" s="73"/>
+      <c r="E38" s="30" t="s">
+        <v>99</v>
+      </c>
+      <c r="F38" s="19" t="s">
+        <v>60</v>
+      </c>
       <c r="G38" s="29"/>
-      <c r="H38" s="29"/>
+      <c r="H38" s="19" t="s">
+        <v>60</v>
+      </c>
       <c r="I38" s="29"/>
       <c r="J38" s="30"/>
       <c r="K38" s="29"/>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A39" s="52">
+        <v>21</v>
+      </c>
+      <c r="B39" s="32" t="s">
+        <v>92</v>
+      </c>
+      <c r="C39" s="51" t="s">
+        <v>41</v>
+      </c>
+      <c r="D39" s="22"/>
+      <c r="E39" s="17"/>
+      <c r="J39" s="17"/>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A40" s="52">
+        <v>22</v>
+      </c>
+      <c r="B40" s="31" t="s">
+        <v>92</v>
+      </c>
+      <c r="C40" s="50" t="s">
+        <v>45</v>
+      </c>
+      <c r="D40" s="27"/>
+      <c r="E40" s="30"/>
+      <c r="F40" s="29"/>
+      <c r="G40" s="29"/>
+      <c r="H40" s="29"/>
+      <c r="I40" s="29"/>
+      <c r="J40" s="30"/>
+      <c r="K40" s="29"/>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A41" s="52">
         <v>23</v>
       </c>
-      <c r="B39" s="31" t="s">
+      <c r="B41" s="31" t="s">
         <v>92</v>
       </c>
-      <c r="C39" s="50" t="s">
+      <c r="C41" s="50" t="s">
+        <v>511</v>
+      </c>
+      <c r="D41" s="27"/>
+      <c r="E41" s="30" t="s">
         <v>512</v>
       </c>
-      <c r="D39" s="27"/>
-      <c r="E39" s="30" t="s">
-        <v>513</v>
-      </c>
-      <c r="F39" s="29"/>
-      <c r="G39" s="55" t="s">
-        <v>516</v>
-      </c>
-      <c r="H39" s="19" t="s">
+      <c r="F41" s="29"/>
+      <c r="G41" s="55" t="s">
+        <v>515</v>
+      </c>
+      <c r="H41" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="I39" s="29"/>
-      <c r="J39" s="30"/>
-      <c r="K39" s="29"/>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="E40" s="15" t="s">
+      <c r="I41" s="29"/>
+      <c r="J41" s="30"/>
+      <c r="K41" s="29"/>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="E42" s="15" t="s">
         <v>89</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="H3:H4"/>
-    <mergeCell ref="I3:I4"/>
-    <mergeCell ref="A3:A9"/>
-    <mergeCell ref="A10:A15"/>
-    <mergeCell ref="A22:A26"/>
-    <mergeCell ref="B3:B9"/>
-    <mergeCell ref="B10:B15"/>
-    <mergeCell ref="B22:B26"/>
-    <mergeCell ref="C35:C36"/>
-    <mergeCell ref="D35:D36"/>
-    <mergeCell ref="C3:C9"/>
-    <mergeCell ref="D3:D9"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="C10:C15"/>
-    <mergeCell ref="D10:D15"/>
-    <mergeCell ref="C22:C26"/>
-    <mergeCell ref="D22:D26"/>
+    <mergeCell ref="H5:H6"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="A5:A11"/>
+    <mergeCell ref="A12:A17"/>
+    <mergeCell ref="A24:A28"/>
+    <mergeCell ref="B5:B11"/>
+    <mergeCell ref="B12:B17"/>
+    <mergeCell ref="B24:B28"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="C5:C11"/>
+    <mergeCell ref="D5:D11"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="C12:C17"/>
+    <mergeCell ref="D12:D17"/>
+    <mergeCell ref="C24:C28"/>
+    <mergeCell ref="D24:D28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3359,6 +3522,115 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18.21875" customWidth="1"/>
+    <col min="2" max="2" width="18" customWidth="1"/>
+    <col min="3" max="3" width="18.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="95" t="s">
+        <v>527</v>
+      </c>
+      <c r="B1" s="95" t="s">
+        <v>529</v>
+      </c>
+      <c r="C1" s="95" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>530</v>
+      </c>
+      <c r="B2" t="s">
+        <v>539</v>
+      </c>
+      <c r="C2" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>526</v>
+      </c>
+      <c r="B3" t="s">
+        <v>112</v>
+      </c>
+      <c r="C3" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>524</v>
+      </c>
+      <c r="B4" t="s">
+        <v>525</v>
+      </c>
+      <c r="C4" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>532</v>
+      </c>
+      <c r="B5" t="s">
+        <v>443</v>
+      </c>
+      <c r="C5" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>534</v>
+      </c>
+      <c r="B6" t="s">
+        <v>535</v>
+      </c>
+      <c r="C6" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>537</v>
+      </c>
+      <c r="B7" t="s">
+        <v>401</v>
+      </c>
+      <c r="C7" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8" t="s">
+        <v>540</v>
+      </c>
+      <c r="C8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="7" tint="0.39997558519241921"/>
@@ -3375,7 +3647,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:A15"/>
   <sheetViews>
@@ -3461,7 +3733,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C16"/>
   <sheetViews>
@@ -3487,7 +3759,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="74" t="s">
+      <c r="A2" s="91" t="s">
         <v>22</v>
       </c>
       <c r="B2">
@@ -3495,61 +3767,61 @@
       </c>
     </row>
     <row r="3" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="74"/>
+      <c r="A3" s="91"/>
       <c r="B3">
         <v>457</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="74"/>
+      <c r="A4" s="91"/>
       <c r="B4">
         <v>473</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="74"/>
+      <c r="A5" s="91"/>
       <c r="B5">
         <v>491</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="74"/>
+      <c r="A6" s="91"/>
       <c r="B6">
         <v>514</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="74"/>
+      <c r="A7" s="91"/>
       <c r="B7">
         <v>532</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="74"/>
+      <c r="A8" s="91"/>
       <c r="B8">
         <v>561</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="74"/>
+      <c r="A9" s="91"/>
       <c r="B9">
         <v>640</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="74"/>
+      <c r="A10" s="91"/>
       <c r="B10">
         <v>660</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="74"/>
+      <c r="A11" s="91"/>
       <c r="B11">
         <v>780</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="74" t="s">
+      <c r="A12" s="91" t="s">
         <v>23</v>
       </c>
       <c r="B12">
@@ -3560,19 +3832,19 @@
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="74"/>
+      <c r="A13" s="91"/>
       <c r="B13">
         <v>830</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="74"/>
+      <c r="A14" s="91"/>
       <c r="B14">
         <v>980</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="74"/>
+      <c r="A15" s="91"/>
       <c r="B15">
         <v>1064</v>
       </c>
@@ -3593,15 +3865,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="8"/>
   </sheetPr>
   <dimension ref="A2:H34"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:G28"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4047,12 +4319,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G147"/>
   <sheetViews>
-    <sheetView topLeftCell="A112" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L151" sqref="L151"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
updates from bb_work branch by @barton RamanCalibration class moved to calibration.py
</commit_message>
<xml_diff>
--- a/documents/Raman data formats.xlsx
+++ b/documents/Raman data formats.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\vm-stor-51\alle\Projekte Kunststoffe\RD\MA\Öffentliche_Projekte\2020-01-07_230007_H2020-CHARISMA_barton\Python\charisma-raman-spectrum-harmonization\documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\vm-stor-51\alle\Projekte Kunststoffe\RD\MA\Öffentliche_Projekte\2020-01-07_230007_H2020-CHARISMA_barton\Python\charisma-development\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52D44DAA-C71A-43F1-8674-A503FB3CA132}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="19308" windowHeight="6660" activeTab="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="File formats" sheetId="6" r:id="rId1"/>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1326" uniqueCount="541">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1326" uniqueCount="542">
   <si>
     <t>Renishaw InVia</t>
   </si>
@@ -1657,11 +1658,14 @@
   <si>
     <t>.0, .1, …</t>
   </si>
+  <si>
+    <t>Can purchase for 2.1k €</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1846,7 +1850,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -1910,6 +1914,71 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1921,7 +1990,7 @@
     <xf numFmtId="0" fontId="17" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="96">
+  <cellXfs count="114">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2120,6 +2189,46 @@
     <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="6" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="0" xfId="7" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="6" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="3" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="4" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -2153,53 +2262,67 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="3" xfId="6" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="4" xfId="6" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="6" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="0" xfId="7" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="4" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="6" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="6" xfId="7" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="7" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="7" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="8" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="9" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="8" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="Gut" xfId="4" builtinId="26"/>
-    <cellStyle name="Hyperlink" xfId="2"/>
+    <cellStyle name="Hyperlink" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="Link" xfId="5" builtinId="8"/>
     <cellStyle name="Neutral" xfId="6" builtinId="28"/>
-    <cellStyle name="Normal 2" xfId="3"/>
+    <cellStyle name="Normal 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
     <cellStyle name="Schlecht" xfId="7" builtinId="27"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
-    <cellStyle name="Standard 2" xfId="1"/>
+    <cellStyle name="Standard 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
   </cellStyles>
   <dxfs count="9">
     <dxf>
@@ -2288,16 +2411,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabelle1" displayName="Tabelle1" ref="A2:G28" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
-  <autoFilter ref="A2:G28"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabelle1" displayName="Tabelle1" ref="A2:G28" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+  <autoFilter ref="A2:G28" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="#" dataDxfId="6"/>
-    <tableColumn id="2" name="Manufacturer name" dataDxfId="5" dataCellStyle="Standard 2"/>
-    <tableColumn id="3" name="Importance (A-D)" dataDxfId="4" dataCellStyle="Standard 2"/>
-    <tableColumn id="4" name="OEM Software Name" dataDxfId="3"/>
-    <tableColumn id="5" name="Extension of native format" dataDxfId="2"/>
-    <tableColumn id="6" name="Python reader available?" dataDxfId="1"/>
-    <tableColumn id="7" name="Test data available ?" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="#" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Manufacturer name" dataDxfId="5" dataCellStyle="Standard 2"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Importance (A-D)" dataDxfId="4" dataCellStyle="Standard 2"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="OEM Software Name" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Extension of native format" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Python reader available?" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Test data available ?" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2565,14 +2688,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
   <dimension ref="A1:K42"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2703,52 +2826,52 @@
       </c>
     </row>
     <row r="5" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="85">
+      <c r="A5" s="80">
         <v>2</v>
       </c>
-      <c r="B5" s="88" t="s">
+      <c r="B5" s="83" t="s">
         <v>90</v>
       </c>
-      <c r="C5" s="74" t="s">
+      <c r="C5" s="88" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="75" t="s">
+      <c r="D5" s="89" t="s">
         <v>26</v>
       </c>
-      <c r="E5" s="78" t="s">
+      <c r="E5" s="92" t="s">
         <v>69</v>
       </c>
-      <c r="F5" s="76" t="s">
+      <c r="F5" s="90" t="s">
         <v>60</v>
       </c>
       <c r="G5" s="56"/>
-      <c r="H5" s="83" t="s">
+      <c r="H5" s="78" t="s">
         <v>516</v>
       </c>
-      <c r="I5" s="83" t="s">
+      <c r="I5" s="78" t="s">
         <v>516</v>
       </c>
       <c r="J5" s="37"/>
       <c r="K5" s="29"/>
     </row>
     <row r="6" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="85"/>
-      <c r="B6" s="88"/>
-      <c r="C6" s="74"/>
-      <c r="D6" s="75"/>
-      <c r="E6" s="78"/>
-      <c r="F6" s="77"/>
+      <c r="A6" s="80"/>
+      <c r="B6" s="83"/>
+      <c r="C6" s="88"/>
+      <c r="D6" s="89"/>
+      <c r="E6" s="92"/>
+      <c r="F6" s="91"/>
       <c r="G6" s="56"/>
-      <c r="H6" s="84"/>
-      <c r="I6" s="84"/>
+      <c r="H6" s="79"/>
+      <c r="I6" s="79"/>
       <c r="J6" s="37"/>
       <c r="K6" s="29"/>
     </row>
     <row r="7" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="85"/>
-      <c r="B7" s="88"/>
-      <c r="C7" s="74"/>
-      <c r="D7" s="75"/>
+      <c r="A7" s="80"/>
+      <c r="B7" s="83"/>
+      <c r="C7" s="88"/>
+      <c r="D7" s="89"/>
       <c r="E7" s="38" t="s">
         <v>70</v>
       </c>
@@ -2768,10 +2891,10 @@
       <c r="K7" s="29"/>
     </row>
     <row r="8" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="85"/>
-      <c r="B8" s="88"/>
-      <c r="C8" s="74"/>
-      <c r="D8" s="75"/>
+      <c r="A8" s="80"/>
+      <c r="B8" s="83"/>
+      <c r="C8" s="88"/>
+      <c r="D8" s="89"/>
       <c r="E8" s="64" t="s">
         <v>71</v>
       </c>
@@ -2789,10 +2912,10 @@
       <c r="K8" s="29"/>
     </row>
     <row r="9" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="85"/>
-      <c r="B9" s="88"/>
-      <c r="C9" s="74"/>
-      <c r="D9" s="75"/>
+      <c r="A9" s="80"/>
+      <c r="B9" s="83"/>
+      <c r="C9" s="88"/>
+      <c r="D9" s="89"/>
       <c r="E9" s="64" t="s">
         <v>72</v>
       </c>
@@ -2807,135 +2930,135 @@
       <c r="J9" s="37"/>
       <c r="K9" s="29"/>
     </row>
-    <row r="10" spans="1:11" s="16" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A10" s="85"/>
-      <c r="B10" s="88"/>
-      <c r="C10" s="74"/>
-      <c r="D10" s="75"/>
-      <c r="E10" s="38" t="s">
+    <row r="10" spans="1:11" s="16" customFormat="1" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="80"/>
+      <c r="B10" s="83"/>
+      <c r="C10" s="88"/>
+      <c r="D10" s="89"/>
+      <c r="E10" s="107" t="s">
         <v>97</v>
       </c>
-      <c r="F10" s="53" t="s">
+      <c r="F10" s="72" t="s">
         <v>60</v>
       </c>
       <c r="G10" s="57" t="s">
         <v>506</v>
       </c>
-      <c r="H10" s="53" t="s">
+      <c r="H10" s="72" t="s">
         <v>60</v>
       </c>
-      <c r="I10" s="53" t="s">
+      <c r="I10" s="72" t="s">
         <v>60</v>
       </c>
       <c r="J10" s="39"/>
       <c r="K10" s="29"/>
     </row>
-    <row r="11" spans="1:11" s="16" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A11" s="85"/>
-      <c r="B11" s="88"/>
-      <c r="C11" s="74"/>
-      <c r="D11" s="75"/>
-      <c r="E11" s="64" t="s">
+    <row r="11" spans="1:11" s="16" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="80"/>
+      <c r="B11" s="83"/>
+      <c r="C11" s="88"/>
+      <c r="D11" s="89"/>
+      <c r="E11" s="111" t="s">
         <v>518</v>
       </c>
-      <c r="F11" s="65" t="s">
+      <c r="F11" s="102" t="s">
         <v>516</v>
       </c>
-      <c r="G11" s="56"/>
-      <c r="H11" s="53" t="s">
+      <c r="G11" s="112"/>
+      <c r="H11" s="104" t="s">
         <v>60</v>
       </c>
-      <c r="I11" s="59" t="s">
+      <c r="I11" s="105" t="s">
         <v>516</v>
       </c>
-      <c r="J11" s="93" t="s">
+      <c r="J11" s="113" t="s">
         <v>520</v>
       </c>
       <c r="K11" s="29"/>
     </row>
-    <row r="12" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="86">
+    <row r="12" spans="1:11" s="16" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="81">
         <v>3</v>
       </c>
-      <c r="B12" s="89" t="s">
+      <c r="B12" s="84" t="s">
         <v>90</v>
       </c>
-      <c r="C12" s="79" t="s">
+      <c r="C12" s="93" t="s">
         <v>15</v>
       </c>
-      <c r="D12" s="80" t="s">
+      <c r="D12" s="94" t="s">
         <v>28</v>
       </c>
-      <c r="E12" s="62" t="s">
+      <c r="E12" s="108" t="s">
         <v>82</v>
       </c>
-      <c r="F12" s="53" t="s">
+      <c r="F12" s="109" t="s">
         <v>60</v>
       </c>
-      <c r="G12" s="58" t="s">
+      <c r="G12" s="110" t="s">
         <v>515</v>
       </c>
-      <c r="H12" s="53" t="s">
+      <c r="H12" s="109" t="s">
         <v>60</v>
       </c>
-      <c r="I12" s="53" t="s">
+      <c r="I12" s="109" t="s">
         <v>60</v>
       </c>
       <c r="J12" s="36"/>
     </row>
-    <row r="13" spans="1:11" s="16" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A13" s="86"/>
-      <c r="B13" s="89"/>
-      <c r="C13" s="79"/>
-      <c r="D13" s="80"/>
-      <c r="E13" s="62" t="s">
+    <row r="13" spans="1:11" s="16" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="81"/>
+      <c r="B13" s="84"/>
+      <c r="C13" s="93"/>
+      <c r="D13" s="94"/>
+      <c r="E13" s="101" t="s">
         <v>77</v>
       </c>
-      <c r="F13" s="65" t="s">
+      <c r="F13" s="102" t="s">
         <v>516</v>
       </c>
-      <c r="G13" s="58"/>
-      <c r="H13" s="53" t="s">
+      <c r="G13" s="103"/>
+      <c r="H13" s="104" t="s">
         <v>60</v>
       </c>
-      <c r="I13" s="59" t="s">
+      <c r="I13" s="105" t="s">
         <v>516</v>
       </c>
-      <c r="J13" s="92" t="s">
-        <v>519</v>
+      <c r="J13" s="106" t="s">
+        <v>541</v>
       </c>
     </row>
     <row r="14" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="86"/>
-      <c r="B14" s="89"/>
-      <c r="C14" s="79"/>
-      <c r="D14" s="80"/>
-      <c r="E14" s="62" t="s">
+      <c r="A14" s="81"/>
+      <c r="B14" s="84"/>
+      <c r="C14" s="93"/>
+      <c r="D14" s="94"/>
+      <c r="E14" s="98" t="s">
         <v>78</v>
       </c>
       <c r="F14" s="65" t="s">
         <v>516</v>
       </c>
-      <c r="G14" s="58"/>
-      <c r="H14" s="53" t="s">
+      <c r="G14" s="99"/>
+      <c r="H14" s="73" t="s">
         <v>60</v>
       </c>
-      <c r="I14" s="59" t="s">
+      <c r="I14" s="100" t="s">
         <v>516</v>
       </c>
-      <c r="J14" s="92" t="s">
+      <c r="J14" s="74" t="s">
         <v>519</v>
       </c>
     </row>
     <row r="15" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="86"/>
-      <c r="B15" s="89"/>
-      <c r="C15" s="79"/>
-      <c r="D15" s="80"/>
+      <c r="A15" s="81"/>
+      <c r="B15" s="84"/>
+      <c r="C15" s="93"/>
+      <c r="D15" s="94"/>
       <c r="E15" s="61" t="s">
         <v>79</v>
       </c>
-      <c r="F15" s="94" t="s">
+      <c r="F15" s="76" t="s">
         <v>516</v>
       </c>
       <c r="G15" s="58"/>
@@ -2948,10 +3071,10 @@
       <c r="J15" s="36"/>
     </row>
     <row r="16" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="86"/>
-      <c r="B16" s="89"/>
-      <c r="C16" s="79"/>
-      <c r="D16" s="80"/>
+      <c r="A16" s="81"/>
+      <c r="B16" s="84"/>
+      <c r="C16" s="93"/>
+      <c r="D16" s="94"/>
       <c r="E16" s="62" t="s">
         <v>80</v>
       </c>
@@ -2970,10 +3093,10 @@
       <c r="J16" s="36"/>
     </row>
     <row r="17" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="86"/>
-      <c r="B17" s="89"/>
-      <c r="C17" s="79"/>
-      <c r="D17" s="80"/>
+      <c r="A17" s="81"/>
+      <c r="B17" s="84"/>
+      <c r="C17" s="93"/>
+      <c r="D17" s="94"/>
       <c r="E17" s="40" t="s">
         <v>81</v>
       </c>
@@ -3050,7 +3173,7 @@
       <c r="I19" s="59" t="s">
         <v>516</v>
       </c>
-      <c r="J19" s="93" t="s">
+      <c r="J19" s="75" t="s">
         <v>521</v>
       </c>
     </row>
@@ -3156,16 +3279,16 @@
       <c r="K23" s="29"/>
     </row>
     <row r="24" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="87">
+      <c r="A24" s="82">
         <v>11</v>
       </c>
-      <c r="B24" s="90" t="s">
+      <c r="B24" s="85" t="s">
         <v>91</v>
       </c>
-      <c r="C24" s="81" t="s">
+      <c r="C24" s="95" t="s">
         <v>64</v>
       </c>
-      <c r="D24" s="82"/>
+      <c r="D24" s="96"/>
       <c r="E24" s="17" t="s">
         <v>88</v>
       </c>
@@ -3175,40 +3298,40 @@
       <c r="J24" s="17"/>
     </row>
     <row r="25" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="87"/>
-      <c r="B25" s="90"/>
-      <c r="C25" s="81"/>
-      <c r="D25" s="82"/>
+      <c r="A25" s="82"/>
+      <c r="B25" s="85"/>
+      <c r="C25" s="95"/>
+      <c r="D25" s="96"/>
       <c r="E25" s="17" t="s">
         <v>84</v>
       </c>
       <c r="J25" s="17"/>
     </row>
     <row r="26" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="87"/>
-      <c r="B26" s="90"/>
-      <c r="C26" s="81"/>
-      <c r="D26" s="82"/>
+      <c r="A26" s="82"/>
+      <c r="B26" s="85"/>
+      <c r="C26" s="95"/>
+      <c r="D26" s="96"/>
       <c r="E26" s="17" t="s">
         <v>85</v>
       </c>
       <c r="J26" s="17"/>
     </row>
     <row r="27" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="87"/>
-      <c r="B27" s="90"/>
-      <c r="C27" s="81"/>
-      <c r="D27" s="82"/>
+      <c r="A27" s="82"/>
+      <c r="B27" s="85"/>
+      <c r="C27" s="95"/>
+      <c r="D27" s="96"/>
       <c r="E27" s="17" t="s">
         <v>86</v>
       </c>
       <c r="J27" s="17"/>
     </row>
     <row r="28" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="87"/>
-      <c r="B28" s="90"/>
-      <c r="C28" s="81"/>
-      <c r="D28" s="82"/>
+      <c r="A28" s="82"/>
+      <c r="B28" s="85"/>
+      <c r="C28" s="95"/>
+      <c r="D28" s="96"/>
       <c r="E28" s="17" t="s">
         <v>87</v>
       </c>
@@ -3394,10 +3517,10 @@
         <v>19</v>
       </c>
       <c r="B37" s="32"/>
-      <c r="C37" s="72" t="s">
+      <c r="C37" s="86" t="s">
         <v>44</v>
       </c>
-      <c r="D37" s="73"/>
+      <c r="D37" s="87"/>
       <c r="E37" s="17" t="s">
         <v>98</v>
       </c>
@@ -3416,8 +3539,8 @@
       <c r="B38" s="31" t="s">
         <v>92</v>
       </c>
-      <c r="C38" s="72"/>
-      <c r="D38" s="73"/>
+      <c r="C38" s="86"/>
+      <c r="D38" s="87"/>
       <c r="E38" s="30" t="s">
         <v>99</v>
       </c>
@@ -3497,14 +3620,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="H5:H6"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="A5:A11"/>
-    <mergeCell ref="A12:A17"/>
-    <mergeCell ref="A24:A28"/>
-    <mergeCell ref="B5:B11"/>
-    <mergeCell ref="B12:B17"/>
-    <mergeCell ref="B24:B28"/>
     <mergeCell ref="C37:C38"/>
     <mergeCell ref="D37:D38"/>
     <mergeCell ref="C5:C11"/>
@@ -3515,6 +3630,14 @@
     <mergeCell ref="D12:D17"/>
     <mergeCell ref="C24:C28"/>
     <mergeCell ref="D24:D28"/>
+    <mergeCell ref="H5:H6"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="A5:A11"/>
+    <mergeCell ref="A12:A17"/>
+    <mergeCell ref="A24:A28"/>
+    <mergeCell ref="B5:B11"/>
+    <mergeCell ref="B12:B17"/>
+    <mergeCell ref="B24:B28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3522,10 +3645,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
@@ -3537,13 +3660,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="95" t="s">
+      <c r="A1" s="77" t="s">
         <v>527</v>
       </c>
-      <c r="B1" s="95" t="s">
+      <c r="B1" s="77" t="s">
         <v>529</v>
       </c>
-      <c r="C1" s="95" t="s">
+      <c r="C1" s="77" t="s">
         <v>528</v>
       </c>
     </row>
@@ -3631,7 +3754,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor theme="7" tint="0.39997558519241921"/>
   </sheetPr>
@@ -3648,7 +3771,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A3:A15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3726,7 +3849,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A3:A17">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:A17">
     <sortCondition ref="A3"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -3734,7 +3857,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3759,7 +3882,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="91" t="s">
+      <c r="A2" s="97" t="s">
         <v>22</v>
       </c>
       <c r="B2">
@@ -3767,61 +3890,61 @@
       </c>
     </row>
     <row r="3" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="91"/>
+      <c r="A3" s="97"/>
       <c r="B3">
         <v>457</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="91"/>
+      <c r="A4" s="97"/>
       <c r="B4">
         <v>473</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="91"/>
+      <c r="A5" s="97"/>
       <c r="B5">
         <v>491</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="91"/>
+      <c r="A6" s="97"/>
       <c r="B6">
         <v>514</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="91"/>
+      <c r="A7" s="97"/>
       <c r="B7">
         <v>532</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="91"/>
+      <c r="A8" s="97"/>
       <c r="B8">
         <v>561</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="91"/>
+      <c r="A9" s="97"/>
       <c r="B9">
         <v>640</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="91"/>
+      <c r="A10" s="97"/>
       <c r="B10">
         <v>660</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="91"/>
+      <c r="A11" s="97"/>
       <c r="B11">
         <v>780</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="91" t="s">
+      <c r="A12" s="97" t="s">
         <v>23</v>
       </c>
       <c r="B12">
@@ -3832,19 +3955,19 @@
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="91"/>
+      <c r="A13" s="97"/>
       <c r="B13">
         <v>830</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="91"/>
+      <c r="A14" s="97"/>
       <c r="B14">
         <v>980</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="91"/>
+      <c r="A15" s="97"/>
       <c r="B15">
         <v>1064</v>
       </c>
@@ -3866,7 +3989,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <tabColor theme="8"/>
   </sheetPr>
@@ -4320,7 +4443,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:G147"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7715,22 +7838,22 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D6" r:id="rId1" location="ftn.table-file-formats-fn1" display="http://gwyddion.net/documentation/user-guide-en/file-formats.html - ftn.table-file-formats-fn1"/>
-    <hyperlink ref="D25" r:id="rId2" location="ftn.table-file-formats-fn1" display="http://gwyddion.net/documentation/user-guide-en/file-formats.html - ftn.table-file-formats-fn1"/>
-    <hyperlink ref="D34" r:id="rId3" location="ftn.table-file-formats-fn2" display="http://gwyddion.net/documentation/user-guide-en/file-formats.html - ftn.table-file-formats-fn2"/>
-    <hyperlink ref="F53" r:id="rId4" location="ftn.table-file-formats-fn3" display="http://gwyddion.net/documentation/user-guide-en/file-formats.html - ftn.table-file-formats-fn3"/>
-    <hyperlink ref="F66" r:id="rId5" location="ftn.table-file-formats-fn3" display="http://gwyddion.net/documentation/user-guide-en/file-formats.html - ftn.table-file-formats-fn3"/>
-    <hyperlink ref="F76" r:id="rId6" location="ftn.table-file-formats-fn3" display="http://gwyddion.net/documentation/user-guide-en/file-formats.html - ftn.table-file-formats-fn3"/>
-    <hyperlink ref="D81" r:id="rId7" location="ftn.table-file-formats-fn4" display="http://gwyddion.net/documentation/user-guide-en/file-formats.html - ftn.table-file-formats-fn4"/>
-    <hyperlink ref="D82" r:id="rId8" location="ftn.table-file-formats-fn5" display="http://gwyddion.net/documentation/user-guide-en/file-formats.html - ftn.table-file-formats-fn5"/>
-    <hyperlink ref="E82" r:id="rId9" location="ftn.table-file-formats-fn6" display="http://gwyddion.net/documentation/user-guide-en/file-formats.html - ftn.table-file-formats-fn6"/>
-    <hyperlink ref="F92" r:id="rId10" location="ftn.table-file-formats-fn3" display="http://gwyddion.net/documentation/user-guide-en/file-formats.html - ftn.table-file-formats-fn3"/>
-    <hyperlink ref="D97" r:id="rId11" location="ftn.table-file-formats-fn7" display="http://gwyddion.net/documentation/user-guide-en/file-formats.html - ftn.table-file-formats-fn7"/>
-    <hyperlink ref="E97" r:id="rId12" location="ftn.table-file-formats-fn8" display="http://gwyddion.net/documentation/user-guide-en/file-formats.html - ftn.table-file-formats-fn8"/>
-    <hyperlink ref="D106" r:id="rId13" location="ftn.table-file-formats-fn9" display="http://gwyddion.net/documentation/user-guide-en/file-formats.html - ftn.table-file-formats-fn9"/>
-    <hyperlink ref="F108" r:id="rId14" location="ftn.table-file-formats-fn3" display="http://gwyddion.net/documentation/user-guide-en/file-formats.html - ftn.table-file-formats-fn3"/>
-    <hyperlink ref="F109" r:id="rId15" location="ftn.table-file-formats-fn3" display="http://gwyddion.net/documentation/user-guide-en/file-formats.html - ftn.table-file-formats-fn3"/>
-    <hyperlink ref="F110" r:id="rId16" location="ftn.table-file-formats-fn3" display="http://gwyddion.net/documentation/user-guide-en/file-formats.html - ftn.table-file-formats-fn3"/>
+    <hyperlink ref="D6" r:id="rId1" location="ftn.table-file-formats-fn1" display="http://gwyddion.net/documentation/user-guide-en/file-formats.html - ftn.table-file-formats-fn1" xr:uid="{00000000-0004-0000-0600-000000000000}"/>
+    <hyperlink ref="D25" r:id="rId2" location="ftn.table-file-formats-fn1" display="http://gwyddion.net/documentation/user-guide-en/file-formats.html - ftn.table-file-formats-fn1" xr:uid="{00000000-0004-0000-0600-000001000000}"/>
+    <hyperlink ref="D34" r:id="rId3" location="ftn.table-file-formats-fn2" display="http://gwyddion.net/documentation/user-guide-en/file-formats.html - ftn.table-file-formats-fn2" xr:uid="{00000000-0004-0000-0600-000002000000}"/>
+    <hyperlink ref="F53" r:id="rId4" location="ftn.table-file-formats-fn3" display="http://gwyddion.net/documentation/user-guide-en/file-formats.html - ftn.table-file-formats-fn3" xr:uid="{00000000-0004-0000-0600-000003000000}"/>
+    <hyperlink ref="F66" r:id="rId5" location="ftn.table-file-formats-fn3" display="http://gwyddion.net/documentation/user-guide-en/file-formats.html - ftn.table-file-formats-fn3" xr:uid="{00000000-0004-0000-0600-000004000000}"/>
+    <hyperlink ref="F76" r:id="rId6" location="ftn.table-file-formats-fn3" display="http://gwyddion.net/documentation/user-guide-en/file-formats.html - ftn.table-file-formats-fn3" xr:uid="{00000000-0004-0000-0600-000005000000}"/>
+    <hyperlink ref="D81" r:id="rId7" location="ftn.table-file-formats-fn4" display="http://gwyddion.net/documentation/user-guide-en/file-formats.html - ftn.table-file-formats-fn4" xr:uid="{00000000-0004-0000-0600-000006000000}"/>
+    <hyperlink ref="D82" r:id="rId8" location="ftn.table-file-formats-fn5" display="http://gwyddion.net/documentation/user-guide-en/file-formats.html - ftn.table-file-formats-fn5" xr:uid="{00000000-0004-0000-0600-000007000000}"/>
+    <hyperlink ref="E82" r:id="rId9" location="ftn.table-file-formats-fn6" display="http://gwyddion.net/documentation/user-guide-en/file-formats.html - ftn.table-file-formats-fn6" xr:uid="{00000000-0004-0000-0600-000008000000}"/>
+    <hyperlink ref="F92" r:id="rId10" location="ftn.table-file-formats-fn3" display="http://gwyddion.net/documentation/user-guide-en/file-formats.html - ftn.table-file-formats-fn3" xr:uid="{00000000-0004-0000-0600-000009000000}"/>
+    <hyperlink ref="D97" r:id="rId11" location="ftn.table-file-formats-fn7" display="http://gwyddion.net/documentation/user-guide-en/file-formats.html - ftn.table-file-formats-fn7" xr:uid="{00000000-0004-0000-0600-00000A000000}"/>
+    <hyperlink ref="E97" r:id="rId12" location="ftn.table-file-formats-fn8" display="http://gwyddion.net/documentation/user-guide-en/file-formats.html - ftn.table-file-formats-fn8" xr:uid="{00000000-0004-0000-0600-00000B000000}"/>
+    <hyperlink ref="D106" r:id="rId13" location="ftn.table-file-formats-fn9" display="http://gwyddion.net/documentation/user-guide-en/file-formats.html - ftn.table-file-formats-fn9" xr:uid="{00000000-0004-0000-0600-00000C000000}"/>
+    <hyperlink ref="F108" r:id="rId14" location="ftn.table-file-formats-fn3" display="http://gwyddion.net/documentation/user-guide-en/file-formats.html - ftn.table-file-formats-fn3" xr:uid="{00000000-0004-0000-0600-00000D000000}"/>
+    <hyperlink ref="F109" r:id="rId15" location="ftn.table-file-formats-fn3" display="http://gwyddion.net/documentation/user-guide-en/file-formats.html - ftn.table-file-formats-fn3" xr:uid="{00000000-0004-0000-0600-00000E000000}"/>
+    <hyperlink ref="F110" r:id="rId16" location="ftn.table-file-formats-fn3" display="http://gwyddion.net/documentation/user-guide-en/file-formats.html - ftn.table-file-formats-fn3" xr:uid="{00000000-0004-0000-0600-00000F000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Latest fixes before D4.3
</commit_message>
<xml_diff>
--- a/documents/Raman data formats.xlsx
+++ b/documents/Raman data formats.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\vm-stor-51\alle\Projekte Kunststoffe\RD\MA\Öffentliche_Projekte\2020-01-07_230007_H2020-CHARISMA_barton\Python\charisma-development\documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\vm-stor-51\alle\Projekte Kunststoffe\RD\MA\Öffentliche_Projekte\2020-01-07_230007_H2020-CHARISMA_barton\Python\charisma-raman-spectrum-harmonization\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52D44DAA-C71A-43F1-8674-A503FB3CA132}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23F134C3-26CE-487D-80FB-41653B5A92A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="9996" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="File formats" sheetId="6" r:id="rId1"/>
@@ -1659,7 +1659,7 @@
     <t>.0, .1, …</t>
   </si>
   <si>
-    <t>Can purchase for 2.1k €</t>
+    <t>purchased</t>
   </si>
 </sst>
 </file>
@@ -2205,6 +2205,87 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="4" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="6" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="7" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="7" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="8" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="9" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="8" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="4" borderId="3" xfId="6" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2229,89 +2310,8 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="4" xfId="7" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="6" xfId="7" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="7" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="7" xfId="7" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="8" xfId="6" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="9" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="8" xfId="7" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -2694,8 +2694,8 @@
   </sheetPr>
   <dimension ref="A1:K42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2826,52 +2826,52 @@
       </c>
     </row>
     <row r="5" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="80">
+      <c r="A5" s="107">
         <v>2</v>
       </c>
-      <c r="B5" s="83" t="s">
+      <c r="B5" s="110" t="s">
         <v>90</v>
       </c>
-      <c r="C5" s="88" t="s">
+      <c r="C5" s="96" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="89" t="s">
+      <c r="D5" s="97" t="s">
         <v>26</v>
       </c>
-      <c r="E5" s="92" t="s">
+      <c r="E5" s="100" t="s">
         <v>69</v>
       </c>
-      <c r="F5" s="90" t="s">
+      <c r="F5" s="98" t="s">
         <v>60</v>
       </c>
       <c r="G5" s="56"/>
-      <c r="H5" s="78" t="s">
+      <c r="H5" s="105" t="s">
         <v>516</v>
       </c>
-      <c r="I5" s="78" t="s">
+      <c r="I5" s="105" t="s">
         <v>516</v>
       </c>
       <c r="J5" s="37"/>
       <c r="K5" s="29"/>
     </row>
     <row r="6" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="80"/>
-      <c r="B6" s="83"/>
-      <c r="C6" s="88"/>
-      <c r="D6" s="89"/>
-      <c r="E6" s="92"/>
-      <c r="F6" s="91"/>
+      <c r="A6" s="107"/>
+      <c r="B6" s="110"/>
+      <c r="C6" s="96"/>
+      <c r="D6" s="97"/>
+      <c r="E6" s="100"/>
+      <c r="F6" s="99"/>
       <c r="G6" s="56"/>
-      <c r="H6" s="79"/>
-      <c r="I6" s="79"/>
+      <c r="H6" s="106"/>
+      <c r="I6" s="106"/>
       <c r="J6" s="37"/>
       <c r="K6" s="29"/>
     </row>
     <row r="7" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="80"/>
-      <c r="B7" s="83"/>
-      <c r="C7" s="88"/>
-      <c r="D7" s="89"/>
+      <c r="A7" s="107"/>
+      <c r="B7" s="110"/>
+      <c r="C7" s="96"/>
+      <c r="D7" s="97"/>
       <c r="E7" s="38" t="s">
         <v>70</v>
       </c>
@@ -2891,10 +2891,10 @@
       <c r="K7" s="29"/>
     </row>
     <row r="8" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="80"/>
-      <c r="B8" s="83"/>
-      <c r="C8" s="88"/>
-      <c r="D8" s="89"/>
+      <c r="A8" s="107"/>
+      <c r="B8" s="110"/>
+      <c r="C8" s="96"/>
+      <c r="D8" s="97"/>
       <c r="E8" s="64" t="s">
         <v>71</v>
       </c>
@@ -2912,10 +2912,10 @@
       <c r="K8" s="29"/>
     </row>
     <row r="9" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="80"/>
-      <c r="B9" s="83"/>
-      <c r="C9" s="88"/>
-      <c r="D9" s="89"/>
+      <c r="A9" s="107"/>
+      <c r="B9" s="110"/>
+      <c r="C9" s="96"/>
+      <c r="D9" s="97"/>
       <c r="E9" s="64" t="s">
         <v>72</v>
       </c>
@@ -2931,11 +2931,11 @@
       <c r="K9" s="29"/>
     </row>
     <row r="10" spans="1:11" s="16" customFormat="1" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="80"/>
-      <c r="B10" s="83"/>
-      <c r="C10" s="88"/>
-      <c r="D10" s="89"/>
-      <c r="E10" s="107" t="s">
+      <c r="A10" s="107"/>
+      <c r="B10" s="110"/>
+      <c r="C10" s="96"/>
+      <c r="D10" s="97"/>
+      <c r="E10" s="87" t="s">
         <v>97</v>
       </c>
       <c r="F10" s="72" t="s">
@@ -2954,96 +2954,96 @@
       <c r="K10" s="29"/>
     </row>
     <row r="11" spans="1:11" s="16" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="80"/>
-      <c r="B11" s="83"/>
-      <c r="C11" s="88"/>
-      <c r="D11" s="89"/>
-      <c r="E11" s="111" t="s">
+      <c r="A11" s="107"/>
+      <c r="B11" s="110"/>
+      <c r="C11" s="96"/>
+      <c r="D11" s="97"/>
+      <c r="E11" s="91" t="s">
         <v>518</v>
       </c>
-      <c r="F11" s="102" t="s">
+      <c r="F11" s="82" t="s">
         <v>516</v>
       </c>
-      <c r="G11" s="112"/>
-      <c r="H11" s="104" t="s">
+      <c r="G11" s="92"/>
+      <c r="H11" s="84" t="s">
         <v>60</v>
       </c>
-      <c r="I11" s="105" t="s">
+      <c r="I11" s="85" t="s">
         <v>516</v>
       </c>
-      <c r="J11" s="113" t="s">
+      <c r="J11" s="93" t="s">
         <v>520</v>
       </c>
       <c r="K11" s="29"/>
     </row>
     <row r="12" spans="1:11" s="16" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="81">
+      <c r="A12" s="108">
         <v>3</v>
       </c>
-      <c r="B12" s="84" t="s">
+      <c r="B12" s="111" t="s">
         <v>90</v>
       </c>
-      <c r="C12" s="93" t="s">
+      <c r="C12" s="101" t="s">
         <v>15</v>
       </c>
-      <c r="D12" s="94" t="s">
+      <c r="D12" s="102" t="s">
         <v>28</v>
       </c>
-      <c r="E12" s="108" t="s">
+      <c r="E12" s="88" t="s">
         <v>82</v>
       </c>
-      <c r="F12" s="109" t="s">
+      <c r="F12" s="89" t="s">
         <v>60</v>
       </c>
-      <c r="G12" s="110" t="s">
+      <c r="G12" s="90" t="s">
         <v>515</v>
       </c>
-      <c r="H12" s="109" t="s">
+      <c r="H12" s="89" t="s">
         <v>60</v>
       </c>
-      <c r="I12" s="109" t="s">
+      <c r="I12" s="89" t="s">
         <v>60</v>
       </c>
       <c r="J12" s="36"/>
     </row>
     <row r="13" spans="1:11" s="16" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="81"/>
-      <c r="B13" s="84"/>
-      <c r="C13" s="93"/>
-      <c r="D13" s="94"/>
-      <c r="E13" s="101" t="s">
+      <c r="A13" s="108"/>
+      <c r="B13" s="111"/>
+      <c r="C13" s="101"/>
+      <c r="D13" s="102"/>
+      <c r="E13" s="81" t="s">
         <v>77</v>
       </c>
-      <c r="F13" s="102" t="s">
+      <c r="F13" s="82" t="s">
         <v>516</v>
       </c>
-      <c r="G13" s="103"/>
-      <c r="H13" s="104" t="s">
+      <c r="G13" s="83"/>
+      <c r="H13" s="84" t="s">
         <v>60</v>
       </c>
-      <c r="I13" s="105" t="s">
-        <v>516</v>
-      </c>
-      <c r="J13" s="106" t="s">
+      <c r="I13" s="84" t="s">
+        <v>60</v>
+      </c>
+      <c r="J13" s="86" t="s">
         <v>541</v>
       </c>
     </row>
     <row r="14" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="81"/>
-      <c r="B14" s="84"/>
-      <c r="C14" s="93"/>
-      <c r="D14" s="94"/>
-      <c r="E14" s="98" t="s">
+      <c r="A14" s="108"/>
+      <c r="B14" s="111"/>
+      <c r="C14" s="101"/>
+      <c r="D14" s="102"/>
+      <c r="E14" s="78" t="s">
         <v>78</v>
       </c>
       <c r="F14" s="65" t="s">
         <v>516</v>
       </c>
-      <c r="G14" s="99"/>
+      <c r="G14" s="79"/>
       <c r="H14" s="73" t="s">
         <v>60</v>
       </c>
-      <c r="I14" s="100" t="s">
+      <c r="I14" s="80" t="s">
         <v>516</v>
       </c>
       <c r="J14" s="74" t="s">
@@ -3051,10 +3051,10 @@
       </c>
     </row>
     <row r="15" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="81"/>
-      <c r="B15" s="84"/>
-      <c r="C15" s="93"/>
-      <c r="D15" s="94"/>
+      <c r="A15" s="108"/>
+      <c r="B15" s="111"/>
+      <c r="C15" s="101"/>
+      <c r="D15" s="102"/>
       <c r="E15" s="61" t="s">
         <v>79</v>
       </c>
@@ -3071,10 +3071,10 @@
       <c r="J15" s="36"/>
     </row>
     <row r="16" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="81"/>
-      <c r="B16" s="84"/>
-      <c r="C16" s="93"/>
-      <c r="D16" s="94"/>
+      <c r="A16" s="108"/>
+      <c r="B16" s="111"/>
+      <c r="C16" s="101"/>
+      <c r="D16" s="102"/>
       <c r="E16" s="62" t="s">
         <v>80</v>
       </c>
@@ -3093,10 +3093,10 @@
       <c r="J16" s="36"/>
     </row>
     <row r="17" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="81"/>
-      <c r="B17" s="84"/>
-      <c r="C17" s="93"/>
-      <c r="D17" s="94"/>
+      <c r="A17" s="108"/>
+      <c r="B17" s="111"/>
+      <c r="C17" s="101"/>
+      <c r="D17" s="102"/>
       <c r="E17" s="40" t="s">
         <v>81</v>
       </c>
@@ -3279,16 +3279,16 @@
       <c r="K23" s="29"/>
     </row>
     <row r="24" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="82">
+      <c r="A24" s="109">
         <v>11</v>
       </c>
-      <c r="B24" s="85" t="s">
+      <c r="B24" s="112" t="s">
         <v>91</v>
       </c>
-      <c r="C24" s="95" t="s">
+      <c r="C24" s="103" t="s">
         <v>64</v>
       </c>
-      <c r="D24" s="96"/>
+      <c r="D24" s="104"/>
       <c r="E24" s="17" t="s">
         <v>88</v>
       </c>
@@ -3298,40 +3298,40 @@
       <c r="J24" s="17"/>
     </row>
     <row r="25" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="82"/>
-      <c r="B25" s="85"/>
-      <c r="C25" s="95"/>
-      <c r="D25" s="96"/>
+      <c r="A25" s="109"/>
+      <c r="B25" s="112"/>
+      <c r="C25" s="103"/>
+      <c r="D25" s="104"/>
       <c r="E25" s="17" t="s">
         <v>84</v>
       </c>
       <c r="J25" s="17"/>
     </row>
     <row r="26" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="82"/>
-      <c r="B26" s="85"/>
-      <c r="C26" s="95"/>
-      <c r="D26" s="96"/>
+      <c r="A26" s="109"/>
+      <c r="B26" s="112"/>
+      <c r="C26" s="103"/>
+      <c r="D26" s="104"/>
       <c r="E26" s="17" t="s">
         <v>85</v>
       </c>
       <c r="J26" s="17"/>
     </row>
     <row r="27" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="82"/>
-      <c r="B27" s="85"/>
-      <c r="C27" s="95"/>
-      <c r="D27" s="96"/>
+      <c r="A27" s="109"/>
+      <c r="B27" s="112"/>
+      <c r="C27" s="103"/>
+      <c r="D27" s="104"/>
       <c r="E27" s="17" t="s">
         <v>86</v>
       </c>
       <c r="J27" s="17"/>
     </row>
     <row r="28" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="82"/>
-      <c r="B28" s="85"/>
-      <c r="C28" s="95"/>
-      <c r="D28" s="96"/>
+      <c r="A28" s="109"/>
+      <c r="B28" s="112"/>
+      <c r="C28" s="103"/>
+      <c r="D28" s="104"/>
       <c r="E28" s="17" t="s">
         <v>87</v>
       </c>
@@ -3517,10 +3517,10 @@
         <v>19</v>
       </c>
       <c r="B37" s="32"/>
-      <c r="C37" s="86" t="s">
+      <c r="C37" s="94" t="s">
         <v>44</v>
       </c>
-      <c r="D37" s="87"/>
+      <c r="D37" s="95"/>
       <c r="E37" s="17" t="s">
         <v>98</v>
       </c>
@@ -3539,8 +3539,8 @@
       <c r="B38" s="31" t="s">
         <v>92</v>
       </c>
-      <c r="C38" s="86"/>
-      <c r="D38" s="87"/>
+      <c r="C38" s="94"/>
+      <c r="D38" s="95"/>
       <c r="E38" s="30" t="s">
         <v>99</v>
       </c>
@@ -3620,6 +3620,14 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="H5:H6"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="A5:A11"/>
+    <mergeCell ref="A12:A17"/>
+    <mergeCell ref="A24:A28"/>
+    <mergeCell ref="B5:B11"/>
+    <mergeCell ref="B12:B17"/>
+    <mergeCell ref="B24:B28"/>
     <mergeCell ref="C37:C38"/>
     <mergeCell ref="D37:D38"/>
     <mergeCell ref="C5:C11"/>
@@ -3630,14 +3638,6 @@
     <mergeCell ref="D12:D17"/>
     <mergeCell ref="C24:C28"/>
     <mergeCell ref="D24:D28"/>
-    <mergeCell ref="H5:H6"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="A5:A11"/>
-    <mergeCell ref="A12:A17"/>
-    <mergeCell ref="A24:A28"/>
-    <mergeCell ref="B5:B11"/>
-    <mergeCell ref="B12:B17"/>
-    <mergeCell ref="B24:B28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3882,7 +3882,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="97" t="s">
+      <c r="A2" s="113" t="s">
         <v>22</v>
       </c>
       <c r="B2">
@@ -3890,61 +3890,61 @@
       </c>
     </row>
     <row r="3" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="97"/>
+      <c r="A3" s="113"/>
       <c r="B3">
         <v>457</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="97"/>
+      <c r="A4" s="113"/>
       <c r="B4">
         <v>473</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="97"/>
+      <c r="A5" s="113"/>
       <c r="B5">
         <v>491</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="97"/>
+      <c r="A6" s="113"/>
       <c r="B6">
         <v>514</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="97"/>
+      <c r="A7" s="113"/>
       <c r="B7">
         <v>532</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="97"/>
+      <c r="A8" s="113"/>
       <c r="B8">
         <v>561</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="97"/>
+      <c r="A9" s="113"/>
       <c r="B9">
         <v>640</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="97"/>
+      <c r="A10" s="113"/>
       <c r="B10">
         <v>660</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="97"/>
+      <c r="A11" s="113"/>
       <c r="B11">
         <v>780</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="97" t="s">
+      <c r="A12" s="113" t="s">
         <v>23</v>
       </c>
       <c r="B12">
@@ -3955,19 +3955,19 @@
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="97"/>
+      <c r="A13" s="113"/>
       <c r="B13">
         <v>830</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="97"/>
+      <c r="A14" s="113"/>
       <c r="B14">
         <v>980</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="97"/>
+      <c r="A15" s="113"/>
       <c r="B15">
         <v>1064</v>
       </c>

</xml_diff>